<commit_message>
updated indexing for excel sheet
</commit_message>
<xml_diff>
--- a/eventDescriptions.xlsx
+++ b/eventDescriptions.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\coup3\Dropbox\Projects\DeathTextWA\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{481FFB26-3858-46C3-B496-49F32325660F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{44D20901-A371-424E-A99C-3B1CADEF0397}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="1" xr2:uid="{08660D2E-95D8-46B6-BECF-03C680FAB143}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="4" xr2:uid="{08660D2E-95D8-46B6-BECF-03C680FAB143}"/>
   </bookViews>
   <sheets>
     <sheet name="SPELL_DAMAGE" sheetId="3" r:id="rId1"/>
@@ -473,21 +473,13 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="10">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -502,195 +494,88 @@
   </cellStyles>
   <dxfs count="80">
     <dxf>
-      <font>
-        <b/>
-      </font>
-      <alignment horizontal="left" vertical="top" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="0" formatCode="General"/>
-      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="0" formatCode="General"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="0" formatCode="General"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="0" formatCode="General"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="0" formatCode="General"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="0" formatCode="General"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="0" formatCode="General"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="0" formatCode="General"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="0" formatCode="General"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="0" formatCode="General"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="0" formatCode="General"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="0" formatCode="General"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="0" formatCode="General"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="0" formatCode="General"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="0" formatCode="General"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="0" formatCode="General"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="0" formatCode="General"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="0" formatCode="General"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="0" formatCode="General"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="0" formatCode="General"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="0" formatCode="General"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="0" formatCode="General"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="0" formatCode="General"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="0" formatCode="General"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="0" formatCode="General"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="0" formatCode="General"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="0" formatCode="General"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="0" formatCode="General"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="0" formatCode="General"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="0" formatCode="General"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="0" formatCode="General"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="0" formatCode="General"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="0" formatCode="General"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="0" formatCode="General"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="0" formatCode="General"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="0" formatCode="General"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="0" formatCode="General"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="0" formatCode="General"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="0" formatCode="General"/>
-    </dxf>
-    <dxf>
-      <border outline="0">
-        <left style="thin">
-          <color theme="1"/>
-        </left>
-        <top style="thin">
-          <color theme="1"/>
-        </top>
-        <bottom style="thin">
-          <color theme="1"/>
-        </bottom>
-      </border>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <name val="Aptos Narrow"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </font>
+      <numFmt numFmtId="0" formatCode="General"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="0" formatCode="General"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="0" formatCode="General"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="0" formatCode="General"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="0" formatCode="General"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="0" formatCode="General"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="0" formatCode="General"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="0" formatCode="General"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="0" formatCode="General"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="0" formatCode="General"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="0" formatCode="General"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="0" formatCode="General"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="0" formatCode="General"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="0" formatCode="General"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="0" formatCode="General"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="0" formatCode="General"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="0" formatCode="General"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="0" formatCode="General"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="0" formatCode="General"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="0" formatCode="General"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="0" formatCode="General"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="0" formatCode="General"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="0" formatCode="General"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="0" formatCode="General"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="0" formatCode="General"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="0" formatCode="General"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="0" formatCode="General"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="0" formatCode="General"/>
     </dxf>
     <dxf>
       <font>
@@ -1321,6 +1206,113 @@
         <vertical/>
         <horizontal/>
       </border>
+    </dxf>
+    <dxf>
+      <border outline="0">
+        <left style="thin">
+          <color theme="1"/>
+        </left>
+        <top style="thin">
+          <color theme="1"/>
+        </top>
+        <bottom style="thin">
+          <color theme="1"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <name val="Aptos Narrow"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+    </dxf>
+    <dxf>
+      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="0" formatCode="General"/>
+      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+      </font>
+      <alignment horizontal="left" vertical="top" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="0" formatCode="General"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="0" formatCode="General"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="0" formatCode="General"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="0" formatCode="General"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="0" formatCode="General"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="0" formatCode="General"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="0" formatCode="General"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="0" formatCode="General"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="0" formatCode="General"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="0" formatCode="General"/>
     </dxf>
     <dxf>
       <numFmt numFmtId="0" formatCode="General"/>
@@ -1377,27 +1369,27 @@
     <filterColumn colId="24" hiddenButton="1"/>
   </autoFilter>
   <tableColumns count="25">
-    <tableColumn id="1" xr3:uid="{0154F10E-2134-42C1-8542-40DB8219A7E3}" name="event" dataDxfId="51"/>
-    <tableColumn id="2" xr3:uid="{EAF9415A-68DE-4451-B3AB-DE24F1760B78}" name="time" dataDxfId="50"/>
-    <tableColumn id="3" xr3:uid="{20B72D57-FA0D-46FC-9AC5-F94DB385B580}" name="subevent" dataDxfId="49"/>
+    <tableColumn id="1" xr3:uid="{0154F10E-2134-42C1-8542-40DB8219A7E3}" name="event" dataDxfId="79"/>
+    <tableColumn id="2" xr3:uid="{EAF9415A-68DE-4451-B3AB-DE24F1760B78}" name="time" dataDxfId="78"/>
+    <tableColumn id="3" xr3:uid="{20B72D57-FA0D-46FC-9AC5-F94DB385B580}" name="subevent" dataDxfId="77"/>
     <tableColumn id="4" xr3:uid="{F623B17F-8423-4ECF-AF58-0963B9DBEF16}" name="hideCaster"/>
-    <tableColumn id="5" xr3:uid="{468A02B9-31A9-4403-A941-ECA29C68D334}" name="sourceGUID" dataDxfId="48"/>
-    <tableColumn id="6" xr3:uid="{6E1EDCD1-0130-4DA1-96DA-26A6774D7A70}" name="sourceName" dataDxfId="47"/>
+    <tableColumn id="5" xr3:uid="{468A02B9-31A9-4403-A941-ECA29C68D334}" name="sourceGUID" dataDxfId="76"/>
+    <tableColumn id="6" xr3:uid="{6E1EDCD1-0130-4DA1-96DA-26A6774D7A70}" name="sourceName" dataDxfId="75"/>
     <tableColumn id="7" xr3:uid="{947B6720-EE48-4A14-9F59-8D336BEA34AA}" name="sourceFlags"/>
     <tableColumn id="8" xr3:uid="{0B33BB71-0EE0-4C73-AF79-36FFC95834EA}" name="sourceRaidFlags"/>
-    <tableColumn id="9" xr3:uid="{4670CDB9-DF72-473E-88CF-4913B9C98915}" name="destGUID" dataDxfId="46"/>
-    <tableColumn id="10" xr3:uid="{5C4CF05F-C6C3-4F40-A7C2-8DFB83CB2173}" name="destName" dataDxfId="45"/>
+    <tableColumn id="9" xr3:uid="{4670CDB9-DF72-473E-88CF-4913B9C98915}" name="destGUID" dataDxfId="74"/>
+    <tableColumn id="10" xr3:uid="{5C4CF05F-C6C3-4F40-A7C2-8DFB83CB2173}" name="destName" dataDxfId="73"/>
     <tableColumn id="11" xr3:uid="{C9D2A499-30EE-4C8C-BEAE-62F68F968035}" name="destFlags"/>
     <tableColumn id="12" xr3:uid="{B27BC529-E967-4B5D-8AAC-7207FF75C82E}" name="destRaidFlags"/>
     <tableColumn id="13" xr3:uid="{7F37A94F-3F6E-44DA-AA97-1F1C9D2B75B0}" name="spellId"/>
-    <tableColumn id="14" xr3:uid="{F9859DFD-77FF-494B-B8A9-31DCB27FF456}" name="spellName" dataDxfId="44"/>
+    <tableColumn id="14" xr3:uid="{F9859DFD-77FF-494B-B8A9-31DCB27FF456}" name="spellName" dataDxfId="72"/>
     <tableColumn id="15" xr3:uid="{E29F758A-B56A-447F-83CD-57C0F68D565E}" name="spellSchool"/>
-    <tableColumn id="16" xr3:uid="{FBE53DA2-7010-4665-B9DF-367B31339E91}" name="amount" dataDxfId="43"/>
-    <tableColumn id="17" xr3:uid="{180C1FA6-3ECD-45DE-ABB1-52687CDF2EF3}" name="overkill" dataDxfId="42"/>
-    <tableColumn id="18" xr3:uid="{5EAF863F-ED33-4DFE-99A8-EBC4C4EA4F1C}" name="school" dataDxfId="41"/>
-    <tableColumn id="19" xr3:uid="{C43C3D52-B987-4BCD-B184-588325A7AA3E}" name="resisted" dataDxfId="40"/>
-    <tableColumn id="20" xr3:uid="{E3813A08-B1BC-4057-A5B6-B29C19B76574}" name="blocked" dataDxfId="39"/>
-    <tableColumn id="21" xr3:uid="{F48D312D-EDF6-49E1-ABC7-D1BD459B538C}" name="absorbed" dataDxfId="38"/>
+    <tableColumn id="16" xr3:uid="{FBE53DA2-7010-4665-B9DF-367B31339E91}" name="amount" dataDxfId="71"/>
+    <tableColumn id="17" xr3:uid="{180C1FA6-3ECD-45DE-ABB1-52687CDF2EF3}" name="overkill" dataDxfId="70"/>
+    <tableColumn id="18" xr3:uid="{5EAF863F-ED33-4DFE-99A8-EBC4C4EA4F1C}" name="school" dataDxfId="69"/>
+    <tableColumn id="19" xr3:uid="{C43C3D52-B987-4BCD-B184-588325A7AA3E}" name="resisted" dataDxfId="68"/>
+    <tableColumn id="20" xr3:uid="{E3813A08-B1BC-4057-A5B6-B29C19B76574}" name="blocked" dataDxfId="67"/>
+    <tableColumn id="21" xr3:uid="{F48D312D-EDF6-49E1-ABC7-D1BD459B538C}" name="absorbed" dataDxfId="66"/>
     <tableColumn id="22" xr3:uid="{1CBBE06F-773A-4866-BD34-24393E10A26D}" name="critical"/>
     <tableColumn id="23" xr3:uid="{7692B4C1-2A9A-4E0F-BF03-7F788E7AE485}" name="glancing"/>
     <tableColumn id="24" xr3:uid="{06F7D4F4-3504-453C-BD68-3E93FE340274}" name="crushing"/>
@@ -1408,21 +1400,21 @@
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="13" xr:uid="{DE86B5F0-54DF-4C35-9E68-A9E9DEC4D00C}" name="Table13" displayName="Table13" ref="A1:F19" headerRowCount="0" totalsRowShown="0" headerRowDxfId="8" dataDxfId="9">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="13" xr:uid="{DE86B5F0-54DF-4C35-9E68-A9E9DEC4D00C}" name="Table13" displayName="Table13" ref="A1:F19" headerRowCount="0" totalsRowShown="0" headerRowDxfId="65" dataDxfId="64">
   <tableColumns count="6">
-    <tableColumn id="1" xr3:uid="{5027B241-393F-4A63-9A76-AFA02DC52634}" name="Column1" headerRowDxfId="2" dataDxfId="0"/>
-    <tableColumn id="2" xr3:uid="{4125EF40-0AC2-46D5-BDC7-7F525CA0B461}" name="Column2" headerRowDxfId="3" dataDxfId="1"/>
-    <tableColumn id="3" xr3:uid="{E35CF92A-5A80-4386-B111-6772B9F1E6CE}" name="Column3" headerRowDxfId="4" dataDxfId="13"/>
-    <tableColumn id="4" xr3:uid="{AA9B68C9-0279-4382-A17D-F7F4DE16A0A4}" name="Column4" headerRowDxfId="5" dataDxfId="12"/>
-    <tableColumn id="5" xr3:uid="{7D2FDEF8-C6D3-43E6-ADEB-005D2D9B3564}" name="Column5" headerRowDxfId="6" dataDxfId="11"/>
-    <tableColumn id="6" xr3:uid="{2FEBF87C-61B6-45BE-90E2-6E7E970081C5}" name="Column6" headerRowDxfId="7" dataDxfId="10"/>
+    <tableColumn id="1" xr3:uid="{5027B241-393F-4A63-9A76-AFA02DC52634}" name="Column1" headerRowDxfId="63" dataDxfId="62"/>
+    <tableColumn id="2" xr3:uid="{4125EF40-0AC2-46D5-BDC7-7F525CA0B461}" name="Column2" headerRowDxfId="61" dataDxfId="60"/>
+    <tableColumn id="3" xr3:uid="{E35CF92A-5A80-4386-B111-6772B9F1E6CE}" name="Column3" headerRowDxfId="59" dataDxfId="58"/>
+    <tableColumn id="4" xr3:uid="{AA9B68C9-0279-4382-A17D-F7F4DE16A0A4}" name="Column4" headerRowDxfId="57" dataDxfId="56"/>
+    <tableColumn id="5" xr3:uid="{7D2FDEF8-C6D3-43E6-ADEB-005D2D9B3564}" name="Column5" headerRowDxfId="55" dataDxfId="54"/>
+    <tableColumn id="6" xr3:uid="{2FEBF87C-61B6-45BE-90E2-6E7E970081C5}" name="Column6" headerRowDxfId="53" dataDxfId="52"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight1" showFirstColumn="0" showLastColumn="0" showRowStripes="0" showColumnStripes="1"/>
 </table>
 </file>
 
 <file path=xl/tables/table3.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="5" xr:uid="{D71C84FC-429D-45FD-AA97-6D4B78140BB9}" name="Table5" displayName="Table5" ref="A1:V9" totalsRowShown="0" dataDxfId="53" tableBorderDxfId="52">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="5" xr:uid="{D71C84FC-429D-45FD-AA97-6D4B78140BB9}" name="Table5" displayName="Table5" ref="A1:V9" totalsRowShown="0" dataDxfId="51" tableBorderDxfId="50">
   <autoFilter ref="A1:V9" xr:uid="{D71C84FC-429D-45FD-AA97-6D4B78140BB9}">
     <filterColumn colId="0" hiddenButton="1"/>
     <filterColumn colId="1" hiddenButton="1"/>
@@ -1448,44 +1440,44 @@
     <filterColumn colId="21" hiddenButton="1"/>
   </autoFilter>
   <tableColumns count="22">
-    <tableColumn id="1" xr3:uid="{5C09FDFC-6B8B-4EFD-AA33-5478A238F88D}" name="event" dataDxfId="75"/>
-    <tableColumn id="2" xr3:uid="{89A8C437-D45D-45AF-9811-78B3F58619CE}" name="time" dataDxfId="74"/>
-    <tableColumn id="3" xr3:uid="{9B290B70-C04A-464F-BE62-79F66A457CFA}" name="subevent" dataDxfId="73"/>
-    <tableColumn id="4" xr3:uid="{A81BC518-2AE7-4996-A532-B0D104860641}" name="hideCaster" dataDxfId="72"/>
-    <tableColumn id="5" xr3:uid="{EC6D5417-797A-4F12-8616-D689F8942579}" name="sourceGUID" dataDxfId="71"/>
-    <tableColumn id="6" xr3:uid="{06453F52-9118-4A35-A14E-285CB77F557F}" name="sourceName" dataDxfId="70"/>
-    <tableColumn id="7" xr3:uid="{E03B4395-5D0F-4CB1-A940-D91F2CC69D12}" name="sourceFlags" dataDxfId="69"/>
-    <tableColumn id="8" xr3:uid="{A88FC6A4-6EB8-471A-83B9-D9BB68934F1B}" name="sourceRaidFlags" dataDxfId="68"/>
-    <tableColumn id="9" xr3:uid="{5E82C048-B304-4DFE-9634-B4642127B617}" name="destGUID" dataDxfId="67"/>
-    <tableColumn id="10" xr3:uid="{ABDDEC54-55AB-42CD-A8A9-B3D2F510569B}" name="destName" dataDxfId="66"/>
-    <tableColumn id="11" xr3:uid="{12103CC7-FA35-4EE0-905C-5CEFA0CE77D8}" name="destFlags" dataDxfId="65"/>
-    <tableColumn id="12" xr3:uid="{2DD45B7F-27AA-4C0B-B553-F59DEDBC9AD4}" name="destRaidFlags" dataDxfId="64"/>
-    <tableColumn id="13" xr3:uid="{551D24FD-8C61-4D01-99E9-D31C4F5EB356}" name="amount" dataDxfId="63"/>
-    <tableColumn id="14" xr3:uid="{1FFB4942-F44F-4A82-93E6-CAE093BDA295}" name="overkill" dataDxfId="62"/>
-    <tableColumn id="15" xr3:uid="{CD4040F6-47E2-4B9C-8EF8-89269CCD51E7}" name="school" dataDxfId="61"/>
-    <tableColumn id="16" xr3:uid="{2F43D450-7B4E-40A0-B53F-B023E73A48D4}" name="resisted" dataDxfId="60"/>
-    <tableColumn id="17" xr3:uid="{B08BD4BE-DAAB-4475-8700-B67CF33E58DA}" name="blocked" dataDxfId="59"/>
-    <tableColumn id="18" xr3:uid="{E745A9D4-D812-4D72-8154-D2CC1DED29C7}" name="absorbed" dataDxfId="58"/>
-    <tableColumn id="19" xr3:uid="{ED756281-2B52-424E-A731-74A651FE5EC3}" name="critical" dataDxfId="57"/>
-    <tableColumn id="20" xr3:uid="{0E38A08F-4882-4F43-8362-CCAF64382E3B}" name="glancing" dataDxfId="56"/>
-    <tableColumn id="21" xr3:uid="{65E13780-54B6-49BF-B3E1-ADB601EA1995}" name="crushing" dataDxfId="55"/>
-    <tableColumn id="22" xr3:uid="{899BDF04-5E82-4240-9236-A33213771375}" name="isOffhand" dataDxfId="54"/>
+    <tableColumn id="1" xr3:uid="{5C09FDFC-6B8B-4EFD-AA33-5478A238F88D}" name="event" dataDxfId="49"/>
+    <tableColumn id="2" xr3:uid="{89A8C437-D45D-45AF-9811-78B3F58619CE}" name="time" dataDxfId="48"/>
+    <tableColumn id="3" xr3:uid="{9B290B70-C04A-464F-BE62-79F66A457CFA}" name="subevent" dataDxfId="47"/>
+    <tableColumn id="4" xr3:uid="{A81BC518-2AE7-4996-A532-B0D104860641}" name="hideCaster" dataDxfId="46"/>
+    <tableColumn id="5" xr3:uid="{EC6D5417-797A-4F12-8616-D689F8942579}" name="sourceGUID" dataDxfId="45"/>
+    <tableColumn id="6" xr3:uid="{06453F52-9118-4A35-A14E-285CB77F557F}" name="sourceName" dataDxfId="44"/>
+    <tableColumn id="7" xr3:uid="{E03B4395-5D0F-4CB1-A940-D91F2CC69D12}" name="sourceFlags" dataDxfId="43"/>
+    <tableColumn id="8" xr3:uid="{A88FC6A4-6EB8-471A-83B9-D9BB68934F1B}" name="sourceRaidFlags" dataDxfId="42"/>
+    <tableColumn id="9" xr3:uid="{5E82C048-B304-4DFE-9634-B4642127B617}" name="destGUID" dataDxfId="41"/>
+    <tableColumn id="10" xr3:uid="{ABDDEC54-55AB-42CD-A8A9-B3D2F510569B}" name="destName" dataDxfId="40"/>
+    <tableColumn id="11" xr3:uid="{12103CC7-FA35-4EE0-905C-5CEFA0CE77D8}" name="destFlags" dataDxfId="39"/>
+    <tableColumn id="12" xr3:uid="{2DD45B7F-27AA-4C0B-B553-F59DEDBC9AD4}" name="destRaidFlags" dataDxfId="38"/>
+    <tableColumn id="13" xr3:uid="{551D24FD-8C61-4D01-99E9-D31C4F5EB356}" name="amount" dataDxfId="37"/>
+    <tableColumn id="14" xr3:uid="{1FFB4942-F44F-4A82-93E6-CAE093BDA295}" name="overkill" dataDxfId="36"/>
+    <tableColumn id="15" xr3:uid="{CD4040F6-47E2-4B9C-8EF8-89269CCD51E7}" name="school" dataDxfId="35"/>
+    <tableColumn id="16" xr3:uid="{2F43D450-7B4E-40A0-B53F-B023E73A48D4}" name="resisted" dataDxfId="34"/>
+    <tableColumn id="17" xr3:uid="{B08BD4BE-DAAB-4475-8700-B67CF33E58DA}" name="blocked" dataDxfId="33"/>
+    <tableColumn id="18" xr3:uid="{E745A9D4-D812-4D72-8154-D2CC1DED29C7}" name="absorbed" dataDxfId="32"/>
+    <tableColumn id="19" xr3:uid="{ED756281-2B52-424E-A731-74A651FE5EC3}" name="critical" dataDxfId="31"/>
+    <tableColumn id="20" xr3:uid="{0E38A08F-4882-4F43-8362-CCAF64382E3B}" name="glancing" dataDxfId="30"/>
+    <tableColumn id="21" xr3:uid="{65E13780-54B6-49BF-B3E1-ADB601EA1995}" name="crushing" dataDxfId="29"/>
+    <tableColumn id="22" xr3:uid="{899BDF04-5E82-4240-9236-A33213771375}" name="isOffhand" dataDxfId="28"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight8" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table4.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{4CE0091E-D941-4896-91B0-021BE146AF9A}" name="Table3" displayName="Table3" ref="A2:C10" totalsRowShown="0" headerRowDxfId="76">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{4CE0091E-D941-4896-91B0-021BE146AF9A}" name="Table3" displayName="Table3" ref="A2:C10" totalsRowShown="0" headerRowDxfId="27">
   <autoFilter ref="A2:C10" xr:uid="{4CE0091E-D941-4896-91B0-021BE146AF9A}">
     <filterColumn colId="0" hiddenButton="1"/>
     <filterColumn colId="1" hiddenButton="1"/>
     <filterColumn colId="2" hiddenButton="1"/>
   </autoFilter>
   <tableColumns count="3">
-    <tableColumn id="1" xr3:uid="{74A3BD8E-4776-4DFE-9362-D55E171A426A}" name="event" dataDxfId="79"/>
-    <tableColumn id="2" xr3:uid="{1D4A90E5-895D-4377-9497-7A520DF6CA5F}" name="unitId" dataDxfId="78"/>
-    <tableColumn id="3" xr3:uid="{19802E2E-C32E-478B-BD12-E4484CF42AAF}" name="?" dataDxfId="77"/>
+    <tableColumn id="1" xr3:uid="{74A3BD8E-4776-4DFE-9362-D55E171A426A}" name="event" dataDxfId="26"/>
+    <tableColumn id="2" xr3:uid="{1D4A90E5-895D-4377-9497-7A520DF6CA5F}" name="unitId" dataDxfId="25"/>
+    <tableColumn id="3" xr3:uid="{19802E2E-C32E-478B-BD12-E4484CF42AAF}" name="?" dataDxfId="24"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight8" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -1510,20 +1502,20 @@
     <filterColumn colId="13" hiddenButton="1"/>
   </autoFilter>
   <tableColumns count="14">
-    <tableColumn id="1" xr3:uid="{55BD533E-5497-48C9-9A3B-9324A93498A3}" name="event" dataDxfId="21"/>
-    <tableColumn id="2" xr3:uid="{1A588E12-DAA6-40F0-A4B4-8F93F78F5A9B}" name="time" dataDxfId="20"/>
-    <tableColumn id="3" xr3:uid="{82794BD6-3D41-404B-92EC-6103DA61636C}" name="subEvent" dataDxfId="19"/>
+    <tableColumn id="1" xr3:uid="{55BD533E-5497-48C9-9A3B-9324A93498A3}" name="event" dataDxfId="23"/>
+    <tableColumn id="2" xr3:uid="{1A588E12-DAA6-40F0-A4B4-8F93F78F5A9B}" name="time" dataDxfId="22"/>
+    <tableColumn id="3" xr3:uid="{82794BD6-3D41-404B-92EC-6103DA61636C}" name="subEvent" dataDxfId="21"/>
     <tableColumn id="4" xr3:uid="{19A45743-437A-4D6D-A09F-357FEDA2AFCA}" name="hideCaster"/>
-    <tableColumn id="5" xr3:uid="{158E90F0-EF2A-4C9E-91F2-6647CF2F3A0C}" name="?" dataDxfId="18"/>
-    <tableColumn id="6" xr3:uid="{44F8D3FF-AC25-44A3-B7FD-00DE91B539AE}" name="?2" dataDxfId="17"/>
+    <tableColumn id="5" xr3:uid="{158E90F0-EF2A-4C9E-91F2-6647CF2F3A0C}" name="?" dataDxfId="20"/>
+    <tableColumn id="6" xr3:uid="{44F8D3FF-AC25-44A3-B7FD-00DE91B539AE}" name="?2" dataDxfId="19"/>
     <tableColumn id="7" xr3:uid="{DDCDD49C-BB24-49D7-A700-E7E12C7EAD6B}" name="?3"/>
     <tableColumn id="8" xr3:uid="{59E7D1CC-D48C-4CB4-9A80-800EEB28891F}" name="?4"/>
-    <tableColumn id="9" xr3:uid="{AE9CA366-1984-4ABE-8030-074227B7B694}" name="sourceGUID" dataDxfId="16"/>
-    <tableColumn id="10" xr3:uid="{F0785829-8642-4408-BAAD-02AB45E856A9}" name="sourceName" dataDxfId="15"/>
+    <tableColumn id="9" xr3:uid="{AE9CA366-1984-4ABE-8030-074227B7B694}" name="sourceGUID" dataDxfId="18"/>
+    <tableColumn id="10" xr3:uid="{F0785829-8642-4408-BAAD-02AB45E856A9}" name="sourceName" dataDxfId="17"/>
     <tableColumn id="11" xr3:uid="{954448AB-5FFA-48C2-8574-1581376DEE1F}" name="sourceFlasg"/>
     <tableColumn id="12" xr3:uid="{F3420589-25E3-4DAA-A588-57BE6122C944}" name="sourceRaidFlags"/>
     <tableColumn id="13" xr3:uid="{C82D2F90-DE7D-4D18-909D-6F44312FB4C0}" name="?5"/>
-    <tableColumn id="14" xr3:uid="{A8B92EE7-18E5-4253-97BE-CF43A49F2F7B}" name="?6" dataDxfId="14"/>
+    <tableColumn id="14" xr3:uid="{A8B92EE7-18E5-4253-97BE-CF43A49F2F7B}" name="?6" dataDxfId="16"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight8" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -1557,29 +1549,29 @@
     <filterColumn colId="22" hiddenButton="1"/>
   </autoFilter>
   <tableColumns count="23">
-    <tableColumn id="1" xr3:uid="{AEBF5E9A-7870-4693-88B2-6F0FCE8E3EB1}" name="event" dataDxfId="37"/>
-    <tableColumn id="2" xr3:uid="{0CFDD8D9-DF05-4707-B269-F9A43BA835CD}" name="time" dataDxfId="36"/>
-    <tableColumn id="3" xr3:uid="{81E017EB-5BC9-4B97-9A0E-352FEB4E4E18}" name="subevent" dataDxfId="35"/>
+    <tableColumn id="1" xr3:uid="{AEBF5E9A-7870-4693-88B2-6F0FCE8E3EB1}" name="event" dataDxfId="15"/>
+    <tableColumn id="2" xr3:uid="{0CFDD8D9-DF05-4707-B269-F9A43BA835CD}" name="time" dataDxfId="14"/>
+    <tableColumn id="3" xr3:uid="{81E017EB-5BC9-4B97-9A0E-352FEB4E4E18}" name="subevent" dataDxfId="13"/>
     <tableColumn id="4" xr3:uid="{603C2070-1BA7-4E19-8CB1-177CFFE6F984}" name="hideCaster"/>
-    <tableColumn id="5" xr3:uid="{A622A293-F794-4688-B998-01D56C0C11A6}" name="sourceGUID" dataDxfId="34"/>
-    <tableColumn id="6" xr3:uid="{DD792953-D842-4633-94AD-68CCAA14045D}" name="sourceName" dataDxfId="33"/>
+    <tableColumn id="5" xr3:uid="{A622A293-F794-4688-B998-01D56C0C11A6}" name="sourceGUID" dataDxfId="12"/>
+    <tableColumn id="6" xr3:uid="{DD792953-D842-4633-94AD-68CCAA14045D}" name="sourceName" dataDxfId="11"/>
     <tableColumn id="7" xr3:uid="{7637BF53-4177-4A19-827D-68A4082E26F5}" name="sourceFlags"/>
     <tableColumn id="8" xr3:uid="{A7927361-9E6D-49DC-967B-FA98560DFD8A}" name="sourceRaidFlags"/>
-    <tableColumn id="9" xr3:uid="{C140D719-F83F-40EC-9E4A-9CF3BC9AC621}" name="destGUID" dataDxfId="32"/>
-    <tableColumn id="10" xr3:uid="{C30CD7F9-A5F2-4071-94E7-80067466767A}" name="destName" dataDxfId="31"/>
+    <tableColumn id="9" xr3:uid="{C140D719-F83F-40EC-9E4A-9CF3BC9AC621}" name="destGUID" dataDxfId="10"/>
+    <tableColumn id="10" xr3:uid="{C30CD7F9-A5F2-4071-94E7-80067466767A}" name="destName" dataDxfId="9"/>
     <tableColumn id="11" xr3:uid="{DF925942-6254-47A5-B937-4D1C5A9BEBE4}" name="destFlags"/>
     <tableColumn id="12" xr3:uid="{68EF1AE4-A436-49A8-8684-393E9ED878C9}" name="destRaidFlags"/>
     <tableColumn id="13" xr3:uid="{DC1E1F75-52F4-461F-8425-35BCA2B4C805}" name="spellId"/>
-    <tableColumn id="14" xr3:uid="{66E1E7E5-098A-4C65-8467-F8A54B3C331E}" name="amount" dataDxfId="30"/>
+    <tableColumn id="14" xr3:uid="{66E1E7E5-098A-4C65-8467-F8A54B3C331E}" name="amount" dataDxfId="8"/>
     <tableColumn id="15" xr3:uid="{C2427716-99AD-49FC-863F-023BEB90008B}" name="overkill"/>
-    <tableColumn id="16" xr3:uid="{356FF27A-7D7F-43A0-A538-4A763368BEC2}" name="school" dataDxfId="29"/>
-    <tableColumn id="17" xr3:uid="{3E5C4CE0-EFC3-4DE4-BE4F-E3C72306041B}" name="?" dataDxfId="28"/>
-    <tableColumn id="18" xr3:uid="{DCD5CBA3-FB16-4AAE-AA23-73D4FC494105}" name="??" dataDxfId="27"/>
-    <tableColumn id="19" xr3:uid="{A518F7DE-34B8-440C-9B27-4A824017B930}" name="???" dataDxfId="26"/>
-    <tableColumn id="20" xr3:uid="{D7F14B74-66C9-479B-A562-BDF1E56299E9}" name="????" dataDxfId="25"/>
-    <tableColumn id="21" xr3:uid="{E533292A-8E02-489C-AD77-66503D319D69}" name="?????" dataDxfId="24"/>
-    <tableColumn id="22" xr3:uid="{BDAFFE2F-4BB6-4697-AF22-EB99872902DF}" name="??????" dataDxfId="23"/>
-    <tableColumn id="23" xr3:uid="{A44B2A08-D4E6-4062-972A-C1055F0BBAF4}" name="???????" dataDxfId="22"/>
+    <tableColumn id="16" xr3:uid="{356FF27A-7D7F-43A0-A538-4A763368BEC2}" name="school" dataDxfId="7"/>
+    <tableColumn id="17" xr3:uid="{3E5C4CE0-EFC3-4DE4-BE4F-E3C72306041B}" name="?" dataDxfId="6"/>
+    <tableColumn id="18" xr3:uid="{DCD5CBA3-FB16-4AAE-AA23-73D4FC494105}" name="??" dataDxfId="5"/>
+    <tableColumn id="19" xr3:uid="{A518F7DE-34B8-440C-9B27-4A824017B930}" name="???" dataDxfId="4"/>
+    <tableColumn id="20" xr3:uid="{D7F14B74-66C9-479B-A562-BDF1E56299E9}" name="????" dataDxfId="3"/>
+    <tableColumn id="21" xr3:uid="{E533292A-8E02-489C-AD77-66503D319D69}" name="?????" dataDxfId="2"/>
+    <tableColumn id="22" xr3:uid="{BDAFFE2F-4BB6-4697-AF22-EB99872902DF}" name="??????" dataDxfId="1"/>
+    <tableColumn id="23" xr3:uid="{A44B2A08-D4E6-4062-972A-C1055F0BBAF4}" name="???????" dataDxfId="0"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight8" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -1991,27 +1983,27 @@
       <c r="Y1" t="s">
         <v>24</v>
       </c>
-      <c r="Z1" s="1" t="s">
+      <c r="Z1" t="s">
         <v>37</v>
       </c>
     </row>
     <row r="2" spans="1:26" x14ac:dyDescent="0.25">
-      <c r="A2" s="1" t="s">
+      <c r="A2" t="s">
         <v>25</v>
       </c>
-      <c r="B2" s="1" t="s">
+      <c r="B2" t="s">
         <v>26</v>
       </c>
-      <c r="C2" s="1" t="s">
+      <c r="C2" t="s">
         <v>27</v>
       </c>
       <c r="D2" t="b">
         <v>0</v>
       </c>
-      <c r="E2" s="1" t="s">
+      <c r="E2" t="s">
         <v>28</v>
       </c>
-      <c r="F2" s="1" t="s">
+      <c r="F2" t="s">
         <v>29</v>
       </c>
       <c r="G2">
@@ -2020,10 +2012,10 @@
       <c r="H2">
         <v>0</v>
       </c>
-      <c r="I2" s="1" t="s">
+      <c r="I2" t="s">
         <v>30</v>
       </c>
-      <c r="J2" s="1" t="s">
+      <c r="J2" t="s">
         <v>31</v>
       </c>
       <c r="K2">
@@ -2035,28 +2027,28 @@
       <c r="M2">
         <v>374045</v>
       </c>
-      <c r="N2" s="1" t="s">
+      <c r="N2" t="s">
         <v>32</v>
       </c>
       <c r="O2">
         <v>64</v>
       </c>
-      <c r="P2" s="1" t="s">
+      <c r="P2" t="s">
         <v>33</v>
       </c>
-      <c r="Q2" s="1" t="s">
+      <c r="Q2" t="s">
         <v>34</v>
       </c>
-      <c r="R2" s="1" t="s">
+      <c r="R2" t="s">
         <v>35</v>
       </c>
-      <c r="S2" s="1" t="s">
-        <v>36</v>
-      </c>
-      <c r="T2" s="1" t="s">
-        <v>36</v>
-      </c>
-      <c r="U2" s="1" t="s">
+      <c r="S2" t="s">
+        <v>36</v>
+      </c>
+      <c r="T2" t="s">
+        <v>36</v>
+      </c>
+      <c r="U2" t="s">
         <v>36</v>
       </c>
       <c r="V2" t="b">
@@ -2071,27 +2063,27 @@
       <c r="Y2" t="b">
         <v>0</v>
       </c>
-      <c r="Z2" s="1" t="s">
+      <c r="Z2" t="s">
         <v>37</v>
       </c>
     </row>
     <row r="3" spans="1:26" x14ac:dyDescent="0.25">
-      <c r="A3" s="1" t="s">
+      <c r="A3" t="s">
         <v>25</v>
       </c>
-      <c r="B3" s="1" t="s">
+      <c r="B3" t="s">
         <v>26</v>
       </c>
-      <c r="C3" s="1" t="s">
+      <c r="C3" t="s">
         <v>27</v>
       </c>
       <c r="D3" t="b">
         <v>0</v>
       </c>
-      <c r="E3" s="1" t="s">
+      <c r="E3" t="s">
         <v>28</v>
       </c>
-      <c r="F3" s="1" t="s">
+      <c r="F3" t="s">
         <v>29</v>
       </c>
       <c r="G3">
@@ -2100,10 +2092,10 @@
       <c r="H3">
         <v>0</v>
       </c>
-      <c r="I3" s="1" t="s">
+      <c r="I3" t="s">
         <v>38</v>
       </c>
-      <c r="J3" s="1" t="s">
+      <c r="J3" t="s">
         <v>39</v>
       </c>
       <c r="K3">
@@ -2115,28 +2107,28 @@
       <c r="M3">
         <v>374045</v>
       </c>
-      <c r="N3" s="1" t="s">
+      <c r="N3" t="s">
         <v>32</v>
       </c>
       <c r="O3">
         <v>64</v>
       </c>
-      <c r="P3" s="1" t="s">
+      <c r="P3" t="s">
         <v>40</v>
       </c>
-      <c r="Q3" s="1" t="s">
+      <c r="Q3" t="s">
         <v>34</v>
       </c>
-      <c r="R3" s="1" t="s">
+      <c r="R3" t="s">
         <v>35</v>
       </c>
-      <c r="S3" s="1" t="s">
-        <v>36</v>
-      </c>
-      <c r="T3" s="1" t="s">
-        <v>36</v>
-      </c>
-      <c r="U3" s="1" t="s">
+      <c r="S3" t="s">
+        <v>36</v>
+      </c>
+      <c r="T3" t="s">
+        <v>36</v>
+      </c>
+      <c r="U3" t="s">
         <v>41</v>
       </c>
       <c r="V3" t="b">
@@ -2151,27 +2143,27 @@
       <c r="Y3" t="b">
         <v>0</v>
       </c>
-      <c r="Z3" s="1" t="s">
+      <c r="Z3" t="s">
         <v>37</v>
       </c>
     </row>
     <row r="4" spans="1:26" x14ac:dyDescent="0.25">
-      <c r="A4" s="1" t="s">
+      <c r="A4" t="s">
         <v>25</v>
       </c>
-      <c r="B4" s="1" t="s">
+      <c r="B4" t="s">
         <v>42</v>
       </c>
-      <c r="C4" s="1" t="s">
+      <c r="C4" t="s">
         <v>43</v>
       </c>
       <c r="D4" t="b">
         <v>0</v>
       </c>
-      <c r="E4" s="1" t="s">
+      <c r="E4" t="s">
         <v>28</v>
       </c>
-      <c r="F4" s="1" t="s">
+      <c r="F4" t="s">
         <v>29</v>
       </c>
       <c r="G4">
@@ -2180,10 +2172,10 @@
       <c r="H4">
         <v>0</v>
       </c>
-      <c r="I4" s="1" t="s">
+      <c r="I4" t="s">
         <v>38</v>
       </c>
-      <c r="J4" s="1" t="s">
+      <c r="J4" t="s">
         <v>39</v>
       </c>
       <c r="K4">
@@ -2195,28 +2187,28 @@
       <c r="M4">
         <v>374020</v>
       </c>
-      <c r="N4" s="1" t="s">
+      <c r="N4" t="s">
         <v>44</v>
       </c>
       <c r="O4">
         <v>64</v>
       </c>
-      <c r="P4" s="1" t="s">
+      <c r="P4" t="s">
         <v>45</v>
       </c>
-      <c r="Q4" s="1" t="s">
+      <c r="Q4" t="s">
         <v>34</v>
       </c>
-      <c r="R4" s="1" t="s">
+      <c r="R4" t="s">
         <v>35</v>
       </c>
-      <c r="S4" s="1" t="s">
-        <v>36</v>
-      </c>
-      <c r="T4" s="1" t="s">
-        <v>36</v>
-      </c>
-      <c r="U4" s="1" t="s">
+      <c r="S4" t="s">
+        <v>36</v>
+      </c>
+      <c r="T4" t="s">
+        <v>36</v>
+      </c>
+      <c r="U4" t="s">
         <v>36</v>
       </c>
       <c r="V4" t="b">
@@ -2231,27 +2223,27 @@
       <c r="Y4" t="b">
         <v>0</v>
       </c>
-      <c r="Z4" s="1" t="s">
+      <c r="Z4" t="s">
         <v>37</v>
       </c>
     </row>
     <row r="5" spans="1:26" x14ac:dyDescent="0.25">
-      <c r="A5" s="1" t="s">
+      <c r="A5" t="s">
         <v>25</v>
       </c>
-      <c r="B5" s="1" t="s">
+      <c r="B5" t="s">
         <v>46</v>
       </c>
-      <c r="C5" s="1" t="s">
+      <c r="C5" t="s">
         <v>43</v>
       </c>
       <c r="D5" t="b">
         <v>0</v>
       </c>
-      <c r="E5" s="1" t="s">
+      <c r="E5" t="s">
         <v>28</v>
       </c>
-      <c r="F5" s="1" t="s">
+      <c r="F5" t="s">
         <v>29</v>
       </c>
       <c r="G5">
@@ -2260,10 +2252,10 @@
       <c r="H5">
         <v>0</v>
       </c>
-      <c r="I5" s="1" t="s">
+      <c r="I5" t="s">
         <v>38</v>
       </c>
-      <c r="J5" s="1" t="s">
+      <c r="J5" t="s">
         <v>39</v>
       </c>
       <c r="K5">
@@ -2275,28 +2267,28 @@
       <c r="M5">
         <v>374020</v>
       </c>
-      <c r="N5" s="1" t="s">
+      <c r="N5" t="s">
         <v>44</v>
       </c>
       <c r="O5">
         <v>64</v>
       </c>
-      <c r="P5" s="1" t="s">
+      <c r="P5" t="s">
         <v>47</v>
       </c>
-      <c r="Q5" s="1" t="s">
+      <c r="Q5" t="s">
         <v>34</v>
       </c>
-      <c r="R5" s="1" t="s">
+      <c r="R5" t="s">
         <v>35</v>
       </c>
-      <c r="S5" s="1" t="s">
-        <v>36</v>
-      </c>
-      <c r="T5" s="1" t="s">
-        <v>36</v>
-      </c>
-      <c r="U5" s="1" t="s">
+      <c r="S5" t="s">
+        <v>36</v>
+      </c>
+      <c r="T5" t="s">
+        <v>36</v>
+      </c>
+      <c r="U5" t="s">
         <v>36</v>
       </c>
       <c r="V5" t="b">
@@ -2311,27 +2303,27 @@
       <c r="Y5" t="b">
         <v>0</v>
       </c>
-      <c r="Z5" s="1" t="s">
+      <c r="Z5" t="s">
         <v>37</v>
       </c>
     </row>
     <row r="6" spans="1:26" x14ac:dyDescent="0.25">
-      <c r="A6" s="1" t="s">
+      <c r="A6" t="s">
         <v>25</v>
       </c>
-      <c r="B6" s="1" t="s">
+      <c r="B6" t="s">
         <v>48</v>
       </c>
-      <c r="C6" s="1" t="s">
+      <c r="C6" t="s">
         <v>43</v>
       </c>
       <c r="D6" t="b">
         <v>0</v>
       </c>
-      <c r="E6" s="1" t="s">
+      <c r="E6" t="s">
         <v>28</v>
       </c>
-      <c r="F6" s="1" t="s">
+      <c r="F6" t="s">
         <v>29</v>
       </c>
       <c r="G6">
@@ -2340,10 +2332,10 @@
       <c r="H6">
         <v>0</v>
       </c>
-      <c r="I6" s="1" t="s">
+      <c r="I6" t="s">
         <v>38</v>
       </c>
-      <c r="J6" s="1" t="s">
+      <c r="J6" t="s">
         <v>39</v>
       </c>
       <c r="K6">
@@ -2355,28 +2347,28 @@
       <c r="M6">
         <v>374020</v>
       </c>
-      <c r="N6" s="1" t="s">
+      <c r="N6" t="s">
         <v>44</v>
       </c>
       <c r="O6">
         <v>64</v>
       </c>
-      <c r="P6" s="1" t="s">
+      <c r="P6" t="s">
         <v>49</v>
       </c>
-      <c r="Q6" s="1" t="s">
+      <c r="Q6" t="s">
         <v>34</v>
       </c>
-      <c r="R6" s="1" t="s">
+      <c r="R6" t="s">
         <v>35</v>
       </c>
-      <c r="S6" s="1" t="s">
-        <v>36</v>
-      </c>
-      <c r="T6" s="1" t="s">
-        <v>36</v>
-      </c>
-      <c r="U6" s="1" t="s">
+      <c r="S6" t="s">
+        <v>36</v>
+      </c>
+      <c r="T6" t="s">
+        <v>36</v>
+      </c>
+      <c r="U6" t="s">
         <v>50</v>
       </c>
       <c r="V6" t="b">
@@ -2391,27 +2383,27 @@
       <c r="Y6" t="b">
         <v>0</v>
       </c>
-      <c r="Z6" s="1" t="s">
+      <c r="Z6" t="s">
         <v>37</v>
       </c>
     </row>
     <row r="7" spans="1:26" x14ac:dyDescent="0.25">
-      <c r="A7" s="1" t="s">
+      <c r="A7" t="s">
         <v>25</v>
       </c>
-      <c r="B7" s="1" t="s">
+      <c r="B7" t="s">
         <v>51</v>
       </c>
-      <c r="C7" s="1" t="s">
+      <c r="C7" t="s">
         <v>43</v>
       </c>
       <c r="D7" t="b">
         <v>0</v>
       </c>
-      <c r="E7" s="1" t="s">
+      <c r="E7" t="s">
         <v>28</v>
       </c>
-      <c r="F7" s="1" t="s">
+      <c r="F7" t="s">
         <v>29</v>
       </c>
       <c r="G7">
@@ -2420,10 +2412,10 @@
       <c r="H7">
         <v>0</v>
       </c>
-      <c r="I7" s="1" t="s">
+      <c r="I7" t="s">
         <v>38</v>
       </c>
-      <c r="J7" s="1" t="s">
+      <c r="J7" t="s">
         <v>39</v>
       </c>
       <c r="K7">
@@ -2435,28 +2427,28 @@
       <c r="M7">
         <v>374020</v>
       </c>
-      <c r="N7" s="1" t="s">
+      <c r="N7" t="s">
         <v>44</v>
       </c>
       <c r="O7">
         <v>64</v>
       </c>
-      <c r="P7" s="1" t="s">
+      <c r="P7" t="s">
         <v>52</v>
       </c>
-      <c r="Q7" s="1" t="s">
+      <c r="Q7" t="s">
         <v>34</v>
       </c>
-      <c r="R7" s="1" t="s">
+      <c r="R7" t="s">
         <v>35</v>
       </c>
-      <c r="S7" s="1" t="s">
-        <v>36</v>
-      </c>
-      <c r="T7" s="1" t="s">
-        <v>36</v>
-      </c>
-      <c r="U7" s="1" t="s">
+      <c r="S7" t="s">
+        <v>36</v>
+      </c>
+      <c r="T7" t="s">
+        <v>36</v>
+      </c>
+      <c r="U7" t="s">
         <v>50</v>
       </c>
       <c r="V7" t="b">
@@ -2471,27 +2463,27 @@
       <c r="Y7" t="b">
         <v>0</v>
       </c>
-      <c r="Z7" s="1" t="s">
+      <c r="Z7" t="s">
         <v>37</v>
       </c>
     </row>
     <row r="8" spans="1:26" x14ac:dyDescent="0.25">
-      <c r="A8" s="1" t="s">
+      <c r="A8" t="s">
         <v>25</v>
       </c>
-      <c r="B8" s="1" t="s">
+      <c r="B8" t="s">
         <v>53</v>
       </c>
-      <c r="C8" s="1" t="s">
+      <c r="C8" t="s">
         <v>43</v>
       </c>
       <c r="D8" t="b">
         <v>0</v>
       </c>
-      <c r="E8" s="1" t="s">
+      <c r="E8" t="s">
         <v>38</v>
       </c>
-      <c r="F8" s="1" t="s">
+      <c r="F8" t="s">
         <v>39</v>
       </c>
       <c r="G8">
@@ -2500,10 +2492,10 @@
       <c r="H8">
         <v>0</v>
       </c>
-      <c r="I8" s="1" t="s">
+      <c r="I8" t="s">
         <v>30</v>
       </c>
-      <c r="J8" s="1" t="s">
+      <c r="J8" t="s">
         <v>31</v>
       </c>
       <c r="K8">
@@ -2515,28 +2507,28 @@
       <c r="M8">
         <v>117952</v>
       </c>
-      <c r="N8" s="1" t="s">
+      <c r="N8" t="s">
         <v>54</v>
       </c>
       <c r="O8">
         <v>8</v>
       </c>
-      <c r="P8" s="1" t="s">
+      <c r="P8" t="s">
         <v>55</v>
       </c>
-      <c r="Q8" s="1" t="s">
+      <c r="Q8" t="s">
         <v>34</v>
       </c>
-      <c r="R8" s="1" t="s">
+      <c r="R8" t="s">
         <v>56</v>
       </c>
-      <c r="S8" s="1" t="s">
-        <v>36</v>
-      </c>
-      <c r="T8" s="1" t="s">
-        <v>36</v>
-      </c>
-      <c r="U8" s="1" t="s">
+      <c r="S8" t="s">
+        <v>36</v>
+      </c>
+      <c r="T8" t="s">
+        <v>36</v>
+      </c>
+      <c r="U8" t="s">
         <v>36</v>
       </c>
       <c r="V8" t="b">
@@ -2551,27 +2543,27 @@
       <c r="Y8" t="b">
         <v>0</v>
       </c>
-      <c r="Z8" s="1" t="s">
+      <c r="Z8" t="s">
         <v>37</v>
       </c>
     </row>
     <row r="9" spans="1:26" x14ac:dyDescent="0.25">
-      <c r="A9" s="1" t="s">
+      <c r="A9" t="s">
         <v>25</v>
       </c>
-      <c r="B9" s="1" t="s">
+      <c r="B9" t="s">
         <v>57</v>
       </c>
-      <c r="C9" s="1" t="s">
+      <c r="C9" t="s">
         <v>43</v>
       </c>
       <c r="D9" t="b">
         <v>0</v>
       </c>
-      <c r="E9" s="1" t="s">
+      <c r="E9" t="s">
         <v>28</v>
       </c>
-      <c r="F9" s="1" t="s">
+      <c r="F9" t="s">
         <v>29</v>
       </c>
       <c r="G9">
@@ -2580,10 +2572,10 @@
       <c r="H9">
         <v>0</v>
       </c>
-      <c r="I9" s="1" t="s">
+      <c r="I9" t="s">
         <v>38</v>
       </c>
-      <c r="J9" s="1" t="s">
+      <c r="J9" t="s">
         <v>39</v>
       </c>
       <c r="K9">
@@ -2595,28 +2587,28 @@
       <c r="M9">
         <v>374020</v>
       </c>
-      <c r="N9" s="1" t="s">
+      <c r="N9" t="s">
         <v>44</v>
       </c>
       <c r="O9">
         <v>64</v>
       </c>
-      <c r="P9" s="1" t="s">
+      <c r="P9" t="s">
         <v>47</v>
       </c>
-      <c r="Q9" s="1" t="s">
+      <c r="Q9" t="s">
         <v>34</v>
       </c>
-      <c r="R9" s="1" t="s">
+      <c r="R9" t="s">
         <v>35</v>
       </c>
-      <c r="S9" s="1" t="s">
-        <v>36</v>
-      </c>
-      <c r="T9" s="1" t="s">
-        <v>36</v>
-      </c>
-      <c r="U9" s="1" t="s">
+      <c r="S9" t="s">
+        <v>36</v>
+      </c>
+      <c r="T9" t="s">
+        <v>36</v>
+      </c>
+      <c r="U9" t="s">
         <v>36</v>
       </c>
       <c r="V9" t="b">
@@ -2631,27 +2623,27 @@
       <c r="Y9" t="b">
         <v>0</v>
       </c>
-      <c r="Z9" s="1" t="s">
+      <c r="Z9" t="s">
         <v>37</v>
       </c>
     </row>
     <row r="10" spans="1:26" x14ac:dyDescent="0.25">
-      <c r="A10" s="1" t="s">
+      <c r="A10" t="s">
         <v>25</v>
       </c>
-      <c r="B10" s="1" t="s">
+      <c r="B10" t="s">
         <v>58</v>
       </c>
-      <c r="C10" s="1" t="s">
+      <c r="C10" t="s">
         <v>43</v>
       </c>
       <c r="D10" t="b">
         <v>0</v>
       </c>
-      <c r="E10" s="1" t="s">
+      <c r="E10" t="s">
         <v>28</v>
       </c>
-      <c r="F10" s="1" t="s">
+      <c r="F10" t="s">
         <v>29</v>
       </c>
       <c r="G10">
@@ -2660,10 +2652,10 @@
       <c r="H10">
         <v>0</v>
       </c>
-      <c r="I10" s="1" t="s">
+      <c r="I10" t="s">
         <v>38</v>
       </c>
-      <c r="J10" s="1" t="s">
+      <c r="J10" t="s">
         <v>39</v>
       </c>
       <c r="K10">
@@ -2675,28 +2667,28 @@
       <c r="M10">
         <v>374020</v>
       </c>
-      <c r="N10" s="1" t="s">
+      <c r="N10" t="s">
         <v>44</v>
       </c>
       <c r="O10">
         <v>64</v>
       </c>
-      <c r="P10" s="1" t="s">
+      <c r="P10" t="s">
         <v>59</v>
       </c>
-      <c r="Q10" s="1" t="s">
+      <c r="Q10" t="s">
         <v>60</v>
       </c>
-      <c r="R10" s="1" t="s">
+      <c r="R10" t="s">
         <v>35</v>
       </c>
-      <c r="S10" s="1" t="s">
-        <v>36</v>
-      </c>
-      <c r="T10" s="1" t="s">
-        <v>36</v>
-      </c>
-      <c r="U10" s="1" t="s">
+      <c r="S10" t="s">
+        <v>36</v>
+      </c>
+      <c r="T10" t="s">
+        <v>36</v>
+      </c>
+      <c r="U10" t="s">
         <v>36</v>
       </c>
       <c r="V10" t="b">
@@ -2713,22 +2705,22 @@
       </c>
     </row>
     <row r="11" spans="1:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A11" s="1">
-        <v>0</v>
-      </c>
-      <c r="B11" s="1">
+      <c r="A11">
+        <v>0</v>
+      </c>
+      <c r="B11">
         <v>1</v>
       </c>
-      <c r="C11" s="1">
+      <c r="C11">
         <v>2</v>
       </c>
       <c r="D11">
         <v>3</v>
       </c>
-      <c r="E11" s="1">
+      <c r="E11">
         <v>4</v>
       </c>
-      <c r="F11" s="1">
+      <c r="F11">
         <v>5</v>
       </c>
       <c r="G11">
@@ -2737,10 +2729,10 @@
       <c r="H11">
         <v>7</v>
       </c>
-      <c r="I11" s="1">
+      <c r="I11">
         <v>8</v>
       </c>
-      <c r="J11" s="1">
+      <c r="J11">
         <v>9</v>
       </c>
       <c r="K11">
@@ -2752,28 +2744,28 @@
       <c r="M11">
         <v>12</v>
       </c>
-      <c r="N11" s="1">
+      <c r="N11">
         <v>14</v>
       </c>
       <c r="O11">
         <v>15</v>
       </c>
-      <c r="P11" s="1">
+      <c r="P11">
         <v>16</v>
       </c>
-      <c r="Q11" s="1">
+      <c r="Q11">
         <v>17</v>
       </c>
-      <c r="R11" s="1">
+      <c r="R11">
         <v>17</v>
       </c>
-      <c r="S11" s="1">
+      <c r="S11">
         <v>18</v>
       </c>
-      <c r="T11" s="1">
+      <c r="T11">
         <v>19</v>
       </c>
-      <c r="U11" s="1">
+      <c r="U11">
         <v>20</v>
       </c>
       <c r="V11">
@@ -2801,399 +2793,399 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{90A3A9AA-6793-4627-9593-A962BC563315}">
   <dimension ref="A1:F20"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="D24" sqref="D24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="21" style="8" bestFit="1" customWidth="1"/>
-    <col min="2" max="6" width="31.42578125" style="6" bestFit="1" customWidth="1"/>
-    <col min="7" max="16384" width="9.140625" style="6"/>
+    <col min="1" max="1" width="21" style="4" bestFit="1" customWidth="1"/>
+    <col min="2" max="6" width="31.42578125" style="3" bestFit="1" customWidth="1"/>
+    <col min="7" max="16384" width="9.140625" style="3"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A1" s="8" t="s">
+      <c r="A1" s="4" t="s">
         <v>99</v>
       </c>
-      <c r="B1" s="6" t="s">
+      <c r="B1" s="3" t="s">
         <v>25</v>
       </c>
-      <c r="C1" s="5" t="s">
+      <c r="C1" s="2" t="s">
         <v>25</v>
       </c>
-      <c r="D1" s="5" t="s">
+      <c r="D1" s="2" t="s">
         <v>25</v>
       </c>
-      <c r="E1" s="5" t="s">
+      <c r="E1" s="2" t="s">
         <v>25</v>
       </c>
-      <c r="F1" s="5" t="s">
+      <c r="F1" s="2" t="s">
         <v>25</v>
       </c>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A2" s="8" t="s">
+      <c r="A2" s="4" t="s">
         <v>100</v>
       </c>
-      <c r="B2" s="6">
+      <c r="B2" s="3">
         <v>1713487394.29</v>
       </c>
-      <c r="C2" s="4">
+      <c r="C2" s="2">
         <v>1713487395.267</v>
       </c>
-      <c r="D2" s="4">
+      <c r="D2" s="2">
         <v>1713487396.2360001</v>
       </c>
-      <c r="E2" s="4">
+      <c r="E2" s="2">
         <v>1713487397.809</v>
       </c>
-      <c r="F2" s="5">
+      <c r="F2" s="2">
         <v>1713487400.016</v>
       </c>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A3" s="8" t="s">
+      <c r="A3" s="4" t="s">
         <v>120</v>
       </c>
-      <c r="B3" s="7" t="s">
+      <c r="B3" s="3" t="s">
         <v>116</v>
       </c>
-      <c r="C3" s="6" t="s">
+      <c r="C3" s="3" t="s">
         <v>116</v>
       </c>
-      <c r="D3" s="6" t="s">
+      <c r="D3" s="3" t="s">
         <v>116</v>
       </c>
-      <c r="E3" s="6" t="s">
+      <c r="E3" s="3" t="s">
         <v>98</v>
       </c>
-      <c r="F3" s="6" t="s">
+      <c r="F3" s="3" t="s">
         <v>98</v>
       </c>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A4" s="8" t="s">
+      <c r="A4" s="4" t="s">
         <v>121</v>
       </c>
-      <c r="B4" s="6" t="b">
-        <v>0</v>
-      </c>
-      <c r="C4" s="6" t="b">
-        <v>0</v>
-      </c>
-      <c r="D4" s="6" t="b">
-        <v>0</v>
-      </c>
-      <c r="E4" s="6" t="b">
-        <v>0</v>
-      </c>
-      <c r="F4" s="6" t="b">
+      <c r="B4" s="3" t="b">
+        <v>0</v>
+      </c>
+      <c r="C4" s="3" t="b">
+        <v>0</v>
+      </c>
+      <c r="D4" s="3" t="b">
+        <v>0</v>
+      </c>
+      <c r="E4" s="3" t="b">
+        <v>0</v>
+      </c>
+      <c r="F4" s="3" t="b">
         <v>0</v>
       </c>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A5" s="8" t="s">
+      <c r="A5" s="4" t="s">
         <v>101</v>
       </c>
-      <c r="B5" s="7" t="s">
+      <c r="B5" s="3" t="s">
         <v>38</v>
       </c>
-      <c r="C5" s="6" t="s">
+      <c r="C5" s="3" t="s">
         <v>38</v>
       </c>
-      <c r="D5" s="6" t="s">
+      <c r="D5" s="3" t="s">
         <v>38</v>
       </c>
-      <c r="E5" s="6" t="s">
+      <c r="E5" s="3" t="s">
         <v>38</v>
       </c>
-      <c r="F5" s="6" t="s">
+      <c r="F5" s="3" t="s">
         <v>38</v>
       </c>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A6" s="8" t="s">
+      <c r="A6" s="4" t="s">
         <v>102</v>
       </c>
-      <c r="B6" s="7" t="s">
+      <c r="B6" s="3" t="s">
         <v>39</v>
       </c>
-      <c r="C6" s="6" t="s">
+      <c r="C6" s="3" t="s">
         <v>39</v>
       </c>
-      <c r="D6" s="6" t="s">
+      <c r="D6" s="3" t="s">
         <v>39</v>
       </c>
-      <c r="E6" s="6" t="s">
+      <c r="E6" s="3" t="s">
         <v>39</v>
       </c>
-      <c r="F6" s="6" t="s">
+      <c r="F6" s="3" t="s">
         <v>39</v>
       </c>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A7" s="8" t="s">
+      <c r="A7" s="4" t="s">
         <v>103</v>
       </c>
-      <c r="B7" s="6">
+      <c r="B7" s="3">
         <v>1297</v>
       </c>
-      <c r="C7" s="6">
+      <c r="C7" s="3">
         <v>1297</v>
       </c>
-      <c r="D7" s="6">
+      <c r="D7" s="3">
         <v>1297</v>
       </c>
-      <c r="E7" s="6">
+      <c r="E7" s="3">
         <v>1297</v>
       </c>
-      <c r="F7" s="6">
+      <c r="F7" s="3">
         <v>1297</v>
       </c>
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A8" s="8" t="s">
+      <c r="A8" s="4" t="s">
         <v>104</v>
       </c>
-      <c r="B8" s="6">
-        <v>0</v>
-      </c>
-      <c r="C8" s="6">
-        <v>0</v>
-      </c>
-      <c r="D8" s="6">
-        <v>0</v>
-      </c>
-      <c r="E8" s="6">
-        <v>0</v>
-      </c>
-      <c r="F8" s="6">
+      <c r="B8" s="3">
+        <v>0</v>
+      </c>
+      <c r="C8" s="3">
+        <v>0</v>
+      </c>
+      <c r="D8" s="3">
+        <v>0</v>
+      </c>
+      <c r="E8" s="3">
+        <v>0</v>
+      </c>
+      <c r="F8" s="3">
         <v>0</v>
       </c>
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A9" s="8" t="s">
+      <c r="A9" s="4" t="s">
         <v>105</v>
       </c>
-      <c r="B9" s="7" t="s">
+      <c r="B9" s="3" t="s">
         <v>38</v>
       </c>
-      <c r="C9" s="6" t="s">
+      <c r="C9" s="3" t="s">
         <v>38</v>
       </c>
-      <c r="D9" s="6" t="s">
+      <c r="D9" s="3" t="s">
         <v>38</v>
       </c>
-      <c r="E9" s="6" t="s">
+      <c r="E9" s="3" t="s">
         <v>38</v>
       </c>
-      <c r="F9" s="6" t="s">
+      <c r="F9" s="3" t="s">
         <v>38</v>
       </c>
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A10" s="8" t="s">
+      <c r="A10" s="4" t="s">
         <v>106</v>
       </c>
-      <c r="B10" s="7" t="s">
+      <c r="B10" s="3" t="s">
         <v>39</v>
       </c>
-      <c r="C10" s="6" t="s">
+      <c r="C10" s="3" t="s">
         <v>39</v>
       </c>
-      <c r="D10" s="6" t="s">
+      <c r="D10" s="3" t="s">
         <v>39</v>
       </c>
-      <c r="E10" s="6" t="s">
+      <c r="E10" s="3" t="s">
         <v>39</v>
       </c>
-      <c r="F10" s="6" t="s">
+      <c r="F10" s="3" t="s">
         <v>39</v>
       </c>
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A11" s="8" t="s">
+      <c r="A11" s="4" t="s">
         <v>107</v>
       </c>
-      <c r="B11" s="6">
+      <c r="B11" s="3">
         <v>1297</v>
       </c>
-      <c r="C11" s="6">
+      <c r="C11" s="3">
         <v>1297</v>
       </c>
-      <c r="D11" s="6">
+      <c r="D11" s="3">
         <v>1297</v>
       </c>
-      <c r="E11" s="6">
+      <c r="E11" s="3">
         <v>1297</v>
       </c>
-      <c r="F11" s="6">
+      <c r="F11" s="3">
         <v>1297</v>
       </c>
     </row>
     <row r="12" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A12" s="8" t="s">
+      <c r="A12" s="4" t="s">
         <v>108</v>
       </c>
-      <c r="B12" s="6">
-        <v>0</v>
-      </c>
-      <c r="C12" s="6">
-        <v>0</v>
-      </c>
-      <c r="D12" s="6">
-        <v>0</v>
-      </c>
-      <c r="E12" s="6">
-        <v>0</v>
-      </c>
-      <c r="F12" s="6">
+      <c r="B12" s="3">
+        <v>0</v>
+      </c>
+      <c r="C12" s="3">
+        <v>0</v>
+      </c>
+      <c r="D12" s="3">
+        <v>0</v>
+      </c>
+      <c r="E12" s="3">
+        <v>0</v>
+      </c>
+      <c r="F12" s="3">
         <v>0</v>
       </c>
     </row>
     <row r="13" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A13" s="8" t="s">
+      <c r="A13" s="4" t="s">
         <v>109</v>
       </c>
-      <c r="B13" s="6">
+      <c r="B13" s="3">
         <v>115175</v>
       </c>
-      <c r="C13" s="6">
+      <c r="C13" s="3">
         <v>115175</v>
       </c>
-      <c r="D13" s="6">
+      <c r="D13" s="3">
         <v>115175</v>
       </c>
-      <c r="E13" s="6">
+      <c r="E13" s="3">
         <v>322101</v>
       </c>
-      <c r="F13" s="6">
+      <c r="F13" s="3">
         <v>116670</v>
       </c>
     </row>
     <row r="14" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A14" s="8" t="s">
+      <c r="A14" s="4" t="s">
         <v>110</v>
       </c>
-      <c r="B14" s="7" t="s">
+      <c r="B14" s="3" t="s">
         <v>117</v>
       </c>
-      <c r="C14" s="6" t="s">
+      <c r="C14" s="3" t="s">
         <v>117</v>
       </c>
-      <c r="D14" s="6" t="s">
+      <c r="D14" s="3" t="s">
         <v>117</v>
       </c>
-      <c r="E14" s="6" t="s">
+      <c r="E14" s="3" t="s">
         <v>118</v>
       </c>
-      <c r="F14" s="6" t="s">
+      <c r="F14" s="3" t="s">
         <v>119</v>
       </c>
     </row>
     <row r="15" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A15" s="8" t="s">
+      <c r="A15" s="4" t="s">
         <v>111</v>
       </c>
-      <c r="B15" s="6">
+      <c r="B15" s="3">
         <v>8</v>
       </c>
-      <c r="C15" s="6">
+      <c r="C15" s="3">
         <v>8</v>
       </c>
-      <c r="D15" s="6">
+      <c r="D15" s="3">
         <v>8</v>
       </c>
-      <c r="E15" s="6">
+      <c r="E15" s="3">
         <v>8</v>
       </c>
-      <c r="F15" s="6">
+      <c r="F15" s="3">
         <v>8</v>
       </c>
     </row>
     <row r="16" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A16" s="8" t="s">
+      <c r="A16" s="4" t="s">
         <v>112</v>
       </c>
-      <c r="B16" s="7">
+      <c r="B16" s="3">
         <v>22147</v>
       </c>
-      <c r="C16" s="6">
+      <c r="C16" s="3">
         <v>22148</v>
       </c>
-      <c r="D16" s="6">
+      <c r="D16" s="3">
         <v>22147</v>
       </c>
-      <c r="E16" s="6">
+      <c r="E16" s="3">
         <v>127878</v>
       </c>
-      <c r="F16" s="6">
+      <c r="F16" s="3">
         <v>129807</v>
       </c>
     </row>
     <row r="17" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A17" s="8" t="s">
+      <c r="A17" s="4" t="s">
         <v>113</v>
       </c>
-      <c r="B17" s="7">
+      <c r="B17" s="3">
         <v>22147</v>
       </c>
-      <c r="C17" s="6">
+      <c r="C17" s="3">
         <v>22148</v>
       </c>
-      <c r="D17" s="6">
+      <c r="D17" s="3">
         <v>22147</v>
       </c>
-      <c r="E17" s="6">
+      <c r="E17" s="3">
         <v>127878</v>
       </c>
-      <c r="F17" s="6">
+      <c r="F17" s="3">
         <v>129807</v>
       </c>
     </row>
     <row r="18" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A18" s="8" t="s">
+      <c r="A18" s="4" t="s">
         <v>114</v>
       </c>
-      <c r="B18" s="7">
-        <v>0</v>
-      </c>
-      <c r="C18" s="6">
-        <v>0</v>
-      </c>
-      <c r="D18" s="6">
-        <v>0</v>
-      </c>
-      <c r="E18" s="6">
-        <v>0</v>
-      </c>
-      <c r="F18" s="6">
+      <c r="B18" s="3">
+        <v>0</v>
+      </c>
+      <c r="C18" s="3">
+        <v>0</v>
+      </c>
+      <c r="D18" s="3">
+        <v>0</v>
+      </c>
+      <c r="E18" s="3">
+        <v>0</v>
+      </c>
+      <c r="F18" s="3">
         <v>0</v>
       </c>
     </row>
     <row r="19" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A19" s="8" t="s">
+      <c r="A19" s="4" t="s">
         <v>115</v>
       </c>
-      <c r="B19" s="7" t="b">
-        <v>0</v>
-      </c>
-      <c r="C19" s="6" t="b">
-        <v>0</v>
-      </c>
-      <c r="D19" s="6" t="b">
-        <v>0</v>
-      </c>
-      <c r="E19" s="6" t="b">
+      <c r="B19" s="3" t="b">
+        <v>0</v>
+      </c>
+      <c r="C19" s="3" t="b">
+        <v>0</v>
+      </c>
+      <c r="D19" s="3" t="b">
+        <v>0</v>
+      </c>
+      <c r="E19" s="3" t="b">
         <v>1</v>
       </c>
-      <c r="F19" s="6" t="b">
+      <c r="F19" s="3" t="b">
         <v>1</v>
       </c>
     </row>
     <row r="20" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A20" s="9"/>
+      <c r="A20" s="5"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -3306,566 +3298,566 @@
       </c>
     </row>
     <row r="2" spans="1:22" x14ac:dyDescent="0.25">
-      <c r="A2" s="3" t="s">
+      <c r="A2" s="1" t="s">
         <v>25</v>
       </c>
-      <c r="B2" s="3" t="s">
+      <c r="B2" s="1" t="s">
         <v>61</v>
       </c>
-      <c r="C2" s="3" t="s">
+      <c r="C2" s="1" t="s">
         <v>62</v>
       </c>
-      <c r="D2" s="2" t="b">
-        <v>0</v>
-      </c>
-      <c r="E2" s="3" t="s">
+      <c r="D2" s="1" t="b">
+        <v>0</v>
+      </c>
+      <c r="E2" s="1" t="s">
         <v>63</v>
       </c>
-      <c r="F2" s="3" t="s">
+      <c r="F2" s="1" t="s">
         <v>64</v>
       </c>
-      <c r="G2" s="2">
+      <c r="G2" s="1">
         <v>2632</v>
       </c>
-      <c r="H2" s="2">
-        <v>0</v>
-      </c>
-      <c r="I2" s="3" t="s">
+      <c r="H2" s="1">
+        <v>0</v>
+      </c>
+      <c r="I2" s="1" t="s">
         <v>65</v>
       </c>
-      <c r="J2" s="3" t="s">
+      <c r="J2" s="1" t="s">
         <v>66</v>
       </c>
-      <c r="K2" s="2">
+      <c r="K2" s="1">
         <v>2632</v>
       </c>
-      <c r="L2" s="2">
-        <v>0</v>
-      </c>
-      <c r="M2" s="2">
+      <c r="L2" s="1">
+        <v>0</v>
+      </c>
+      <c r="M2" s="1">
         <v>71652</v>
       </c>
-      <c r="N2" s="3" t="s">
+      <c r="N2" s="1" t="s">
         <v>34</v>
       </c>
-      <c r="O2" s="2">
+      <c r="O2" s="1">
         <v>1</v>
       </c>
-      <c r="P2" s="3" t="s">
-        <v>36</v>
-      </c>
-      <c r="Q2" s="3" t="s">
-        <v>36</v>
-      </c>
-      <c r="R2" s="3" t="s">
-        <v>36</v>
-      </c>
-      <c r="S2" s="3" t="s">
+      <c r="P2" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="Q2" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="R2" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="S2" s="1" t="s">
         <v>67</v>
       </c>
-      <c r="T2" s="3" t="s">
+      <c r="T2" s="1" t="s">
         <v>67</v>
       </c>
-      <c r="U2" s="3" t="s">
+      <c r="U2" s="1" t="s">
         <v>67</v>
       </c>
-      <c r="V2" s="2" t="b">
+      <c r="V2" s="1" t="b">
         <v>0</v>
       </c>
     </row>
     <row r="3" spans="1:22" x14ac:dyDescent="0.25">
-      <c r="A3" s="3" t="s">
+      <c r="A3" s="1" t="s">
         <v>25</v>
       </c>
-      <c r="B3" s="3" t="s">
+      <c r="B3" s="1" t="s">
         <v>68</v>
       </c>
-      <c r="C3" s="3" t="s">
+      <c r="C3" s="1" t="s">
         <v>62</v>
       </c>
-      <c r="D3" s="2" t="b">
-        <v>0</v>
-      </c>
-      <c r="E3" s="3" t="s">
+      <c r="D3" s="1" t="b">
+        <v>0</v>
+      </c>
+      <c r="E3" s="1" t="s">
         <v>30</v>
       </c>
-      <c r="F3" s="3" t="s">
+      <c r="F3" s="1" t="s">
         <v>31</v>
       </c>
-      <c r="G3" s="2">
+      <c r="G3" s="1">
         <v>68168</v>
       </c>
-      <c r="H3" s="2">
-        <v>0</v>
-      </c>
-      <c r="I3" s="3" t="s">
+      <c r="H3" s="1">
+        <v>0</v>
+      </c>
+      <c r="I3" s="1" t="s">
         <v>38</v>
       </c>
-      <c r="J3" s="3" t="s">
+      <c r="J3" s="1" t="s">
         <v>39</v>
       </c>
-      <c r="K3" s="2">
+      <c r="K3" s="1">
         <v>1297</v>
       </c>
-      <c r="L3" s="2">
-        <v>0</v>
-      </c>
-      <c r="M3" s="2">
+      <c r="L3" s="1">
+        <v>0</v>
+      </c>
+      <c r="M3" s="1">
         <v>83101</v>
       </c>
-      <c r="N3" s="3" t="s">
+      <c r="N3" s="1" t="s">
         <v>34</v>
       </c>
-      <c r="O3" s="2">
+      <c r="O3" s="1">
         <v>1</v>
       </c>
-      <c r="P3" s="3" t="s">
-        <v>36</v>
-      </c>
-      <c r="Q3" s="3" t="s">
-        <v>36</v>
-      </c>
-      <c r="R3" s="3" t="s">
-        <v>36</v>
-      </c>
-      <c r="S3" s="3" t="s">
+      <c r="P3" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="Q3" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="R3" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="S3" s="1" t="s">
         <v>67</v>
       </c>
-      <c r="T3" s="3" t="s">
+      <c r="T3" s="1" t="s">
         <v>67</v>
       </c>
-      <c r="U3" s="3" t="s">
+      <c r="U3" s="1" t="s">
         <v>67</v>
       </c>
-      <c r="V3" s="2" t="b">
+      <c r="V3" s="1" t="b">
         <v>0</v>
       </c>
     </row>
     <row r="4" spans="1:22" x14ac:dyDescent="0.25">
-      <c r="A4" s="3" t="s">
+      <c r="A4" s="1" t="s">
         <v>25</v>
       </c>
-      <c r="B4" s="3" t="s">
+      <c r="B4" s="1" t="s">
         <v>69</v>
       </c>
-      <c r="C4" s="3" t="s">
+      <c r="C4" s="1" t="s">
         <v>62</v>
       </c>
-      <c r="D4" s="2" t="b">
-        <v>0</v>
-      </c>
-      <c r="E4" s="3" t="s">
+      <c r="D4" s="1" t="b">
+        <v>0</v>
+      </c>
+      <c r="E4" s="1" t="s">
         <v>63</v>
       </c>
-      <c r="F4" s="3" t="s">
+      <c r="F4" s="1" t="s">
         <v>64</v>
       </c>
-      <c r="G4" s="2">
+      <c r="G4" s="1">
         <v>2632</v>
       </c>
-      <c r="H4" s="2">
-        <v>0</v>
-      </c>
-      <c r="I4" s="3" t="s">
+      <c r="H4" s="1">
+        <v>0</v>
+      </c>
+      <c r="I4" s="1" t="s">
         <v>65</v>
       </c>
-      <c r="J4" s="3" t="s">
+      <c r="J4" s="1" t="s">
         <v>66</v>
       </c>
-      <c r="K4" s="2">
+      <c r="K4" s="1">
         <v>2632</v>
       </c>
-      <c r="L4" s="2">
-        <v>0</v>
-      </c>
-      <c r="M4" s="2">
+      <c r="L4" s="1">
+        <v>0</v>
+      </c>
+      <c r="M4" s="1">
         <v>37299</v>
       </c>
-      <c r="N4" s="3" t="s">
+      <c r="N4" s="1" t="s">
         <v>34</v>
       </c>
-      <c r="O4" s="2">
+      <c r="O4" s="1">
         <v>1</v>
       </c>
-      <c r="P4" s="3" t="s">
-        <v>36</v>
-      </c>
-      <c r="Q4" s="3" t="s">
-        <v>36</v>
-      </c>
-      <c r="R4" s="3" t="s">
-        <v>36</v>
-      </c>
-      <c r="S4" s="3" t="s">
+      <c r="P4" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="Q4" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="R4" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="S4" s="1" t="s">
         <v>67</v>
       </c>
-      <c r="T4" s="3" t="s">
+      <c r="T4" s="1" t="s">
         <v>67</v>
       </c>
-      <c r="U4" s="3" t="s">
+      <c r="U4" s="1" t="s">
         <v>67</v>
       </c>
-      <c r="V4" s="2" t="b">
+      <c r="V4" s="1" t="b">
         <v>1</v>
       </c>
     </row>
     <row r="5" spans="1:22" x14ac:dyDescent="0.25">
-      <c r="A5" s="3" t="s">
+      <c r="A5" s="1" t="s">
         <v>25</v>
       </c>
-      <c r="B5" s="3" t="s">
+      <c r="B5" s="1" t="s">
         <v>70</v>
       </c>
-      <c r="C5" s="3" t="s">
+      <c r="C5" s="1" t="s">
         <v>62</v>
       </c>
-      <c r="D5" s="2" t="b">
-        <v>0</v>
-      </c>
-      <c r="E5" s="3" t="s">
+      <c r="D5" s="1" t="b">
+        <v>0</v>
+      </c>
+      <c r="E5" s="1" t="s">
         <v>63</v>
       </c>
-      <c r="F5" s="3" t="s">
+      <c r="F5" s="1" t="s">
         <v>64</v>
       </c>
-      <c r="G5" s="2">
+      <c r="G5" s="1">
         <v>2632</v>
       </c>
-      <c r="H5" s="2">
-        <v>0</v>
-      </c>
-      <c r="I5" s="3" t="s">
+      <c r="H5" s="1">
+        <v>0</v>
+      </c>
+      <c r="I5" s="1" t="s">
         <v>65</v>
       </c>
-      <c r="J5" s="3" t="s">
+      <c r="J5" s="1" t="s">
         <v>66</v>
       </c>
-      <c r="K5" s="2">
+      <c r="K5" s="1">
         <v>2632</v>
       </c>
-      <c r="L5" s="2">
-        <v>0</v>
-      </c>
-      <c r="M5" s="2">
+      <c r="L5" s="1">
+        <v>0</v>
+      </c>
+      <c r="M5" s="1">
         <v>73043</v>
       </c>
-      <c r="N5" s="3" t="s">
+      <c r="N5" s="1" t="s">
         <v>34</v>
       </c>
-      <c r="O5" s="2">
+      <c r="O5" s="1">
         <v>1</v>
       </c>
-      <c r="P5" s="3" t="s">
-        <v>36</v>
-      </c>
-      <c r="Q5" s="3" t="s">
-        <v>36</v>
-      </c>
-      <c r="R5" s="3" t="s">
-        <v>36</v>
-      </c>
-      <c r="S5" s="3" t="s">
+      <c r="P5" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="Q5" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="R5" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="S5" s="1" t="s">
         <v>67</v>
       </c>
-      <c r="T5" s="3" t="s">
+      <c r="T5" s="1" t="s">
         <v>67</v>
       </c>
-      <c r="U5" s="3" t="s">
+      <c r="U5" s="1" t="s">
         <v>67</v>
       </c>
-      <c r="V5" s="2" t="b">
+      <c r="V5" s="1" t="b">
         <v>0</v>
       </c>
     </row>
     <row r="6" spans="1:22" x14ac:dyDescent="0.25">
-      <c r="A6" s="3" t="s">
+      <c r="A6" s="1" t="s">
         <v>25</v>
       </c>
-      <c r="B6" s="3" t="s">
+      <c r="B6" s="1" t="s">
         <v>71</v>
       </c>
-      <c r="C6" s="3" t="s">
+      <c r="C6" s="1" t="s">
         <v>62</v>
       </c>
-      <c r="D6" s="2" t="b">
-        <v>0</v>
-      </c>
-      <c r="E6" s="3" t="s">
+      <c r="D6" s="1" t="b">
+        <v>0</v>
+      </c>
+      <c r="E6" s="1" t="s">
         <v>63</v>
       </c>
-      <c r="F6" s="3" t="s">
+      <c r="F6" s="1" t="s">
         <v>64</v>
       </c>
-      <c r="G6" s="2">
+      <c r="G6" s="1">
         <v>2632</v>
       </c>
-      <c r="H6" s="2">
-        <v>0</v>
-      </c>
-      <c r="I6" s="3" t="s">
+      <c r="H6" s="1">
+        <v>0</v>
+      </c>
+      <c r="I6" s="1" t="s">
         <v>65</v>
       </c>
-      <c r="J6" s="3" t="s">
+      <c r="J6" s="1" t="s">
         <v>66</v>
       </c>
-      <c r="K6" s="2">
+      <c r="K6" s="1">
         <v>2632</v>
       </c>
-      <c r="L6" s="2">
-        <v>0</v>
-      </c>
-      <c r="M6" s="2">
+      <c r="L6" s="1">
+        <v>0</v>
+      </c>
+      <c r="M6" s="1">
         <v>36374</v>
       </c>
-      <c r="N6" s="3" t="s">
+      <c r="N6" s="1" t="s">
         <v>34</v>
       </c>
-      <c r="O6" s="2">
+      <c r="O6" s="1">
         <v>1</v>
       </c>
-      <c r="P6" s="3" t="s">
-        <v>36</v>
-      </c>
-      <c r="Q6" s="3" t="s">
-        <v>36</v>
-      </c>
-      <c r="R6" s="3" t="s">
-        <v>36</v>
-      </c>
-      <c r="S6" s="3" t="s">
+      <c r="P6" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="Q6" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="R6" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="S6" s="1" t="s">
         <v>67</v>
       </c>
-      <c r="T6" s="3" t="s">
+      <c r="T6" s="1" t="s">
         <v>67</v>
       </c>
-      <c r="U6" s="3" t="s">
+      <c r="U6" s="1" t="s">
         <v>67</v>
       </c>
-      <c r="V6" s="2" t="b">
+      <c r="V6" s="1" t="b">
         <v>1</v>
       </c>
     </row>
     <row r="7" spans="1:22" x14ac:dyDescent="0.25">
-      <c r="A7" s="3" t="s">
+      <c r="A7" s="1" t="s">
         <v>25</v>
       </c>
-      <c r="B7" s="3" t="s">
+      <c r="B7" s="1" t="s">
         <v>72</v>
       </c>
-      <c r="C7" s="3" t="s">
+      <c r="C7" s="1" t="s">
         <v>62</v>
       </c>
-      <c r="D7" s="2" t="b">
-        <v>0</v>
-      </c>
-      <c r="E7" s="3" t="s">
+      <c r="D7" s="1" t="b">
+        <v>0</v>
+      </c>
+      <c r="E7" s="1" t="s">
         <v>63</v>
       </c>
-      <c r="F7" s="3" t="s">
+      <c r="F7" s="1" t="s">
         <v>64</v>
       </c>
-      <c r="G7" s="2">
+      <c r="G7" s="1">
         <v>2632</v>
       </c>
-      <c r="H7" s="2">
-        <v>0</v>
-      </c>
-      <c r="I7" s="3" t="s">
+      <c r="H7" s="1">
+        <v>0</v>
+      </c>
+      <c r="I7" s="1" t="s">
         <v>65</v>
       </c>
-      <c r="J7" s="3" t="s">
+      <c r="J7" s="1" t="s">
         <v>66</v>
       </c>
-      <c r="K7" s="2">
+      <c r="K7" s="1">
         <v>2632</v>
       </c>
-      <c r="L7" s="2">
-        <v>0</v>
-      </c>
-      <c r="M7" s="2">
+      <c r="L7" s="1">
+        <v>0</v>
+      </c>
+      <c r="M7" s="1">
         <v>68899</v>
       </c>
-      <c r="N7" s="3" t="s">
+      <c r="N7" s="1" t="s">
         <v>34</v>
       </c>
-      <c r="O7" s="2">
+      <c r="O7" s="1">
         <v>1</v>
       </c>
-      <c r="P7" s="3" t="s">
-        <v>36</v>
-      </c>
-      <c r="Q7" s="3" t="s">
-        <v>36</v>
-      </c>
-      <c r="R7" s="3" t="s">
-        <v>36</v>
-      </c>
-      <c r="S7" s="3" t="s">
+      <c r="P7" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="Q7" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="R7" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="S7" s="1" t="s">
         <v>67</v>
       </c>
-      <c r="T7" s="3" t="s">
+      <c r="T7" s="1" t="s">
         <v>67</v>
       </c>
-      <c r="U7" s="3" t="s">
+      <c r="U7" s="1" t="s">
         <v>67</v>
       </c>
-      <c r="V7" s="2" t="b">
+      <c r="V7" s="1" t="b">
         <v>0</v>
       </c>
     </row>
     <row r="8" spans="1:22" x14ac:dyDescent="0.25">
-      <c r="A8" s="3" t="s">
+      <c r="A8" s="1" t="s">
         <v>25</v>
       </c>
-      <c r="B8" s="3" t="s">
+      <c r="B8" s="1" t="s">
         <v>73</v>
       </c>
-      <c r="C8" s="3" t="s">
+      <c r="C8" s="1" t="s">
         <v>62</v>
       </c>
-      <c r="D8" s="2" t="b">
-        <v>0</v>
-      </c>
-      <c r="E8" s="3" t="s">
+      <c r="D8" s="1" t="b">
+        <v>0</v>
+      </c>
+      <c r="E8" s="1" t="s">
         <v>30</v>
       </c>
-      <c r="F8" s="3" t="s">
+      <c r="F8" s="1" t="s">
         <v>31</v>
       </c>
-      <c r="G8" s="2">
+      <c r="G8" s="1">
         <v>68168</v>
       </c>
-      <c r="H8" s="2">
-        <v>0</v>
-      </c>
-      <c r="I8" s="3" t="s">
+      <c r="H8" s="1">
+        <v>0</v>
+      </c>
+      <c r="I8" s="1" t="s">
         <v>38</v>
       </c>
-      <c r="J8" s="3" t="s">
+      <c r="J8" s="1" t="s">
         <v>39</v>
       </c>
-      <c r="K8" s="2">
+      <c r="K8" s="1">
         <v>1297</v>
       </c>
-      <c r="L8" s="2">
-        <v>0</v>
-      </c>
-      <c r="M8" s="2">
+      <c r="L8" s="1">
+        <v>0</v>
+      </c>
+      <c r="M8" s="1">
         <v>82168</v>
       </c>
-      <c r="N8" s="3" t="s">
+      <c r="N8" s="1" t="s">
         <v>34</v>
       </c>
-      <c r="O8" s="2">
+      <c r="O8" s="1">
         <v>1</v>
       </c>
-      <c r="P8" s="3" t="s">
-        <v>36</v>
-      </c>
-      <c r="Q8" s="3" t="s">
-        <v>36</v>
-      </c>
-      <c r="R8" s="3" t="s">
-        <v>36</v>
-      </c>
-      <c r="S8" s="3" t="s">
+      <c r="P8" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="Q8" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="R8" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="S8" s="1" t="s">
         <v>67</v>
       </c>
-      <c r="T8" s="3" t="s">
+      <c r="T8" s="1" t="s">
         <v>67</v>
       </c>
-      <c r="U8" s="3" t="s">
+      <c r="U8" s="1" t="s">
         <v>67</v>
       </c>
-      <c r="V8" s="2" t="b">
+      <c r="V8" s="1" t="b">
         <v>0</v>
       </c>
     </row>
     <row r="9" spans="1:22" x14ac:dyDescent="0.25">
-      <c r="A9" s="3" t="s">
+      <c r="A9" s="1" t="s">
         <v>25</v>
       </c>
-      <c r="B9" s="3" t="s">
+      <c r="B9" s="1" t="s">
         <v>74</v>
       </c>
-      <c r="C9" s="3" t="s">
+      <c r="C9" s="1" t="s">
         <v>62</v>
       </c>
-      <c r="D9" s="2" t="b">
-        <v>0</v>
-      </c>
-      <c r="E9" s="3" t="s">
+      <c r="D9" s="1" t="b">
+        <v>0</v>
+      </c>
+      <c r="E9" s="1" t="s">
         <v>63</v>
       </c>
-      <c r="F9" s="3" t="s">
+      <c r="F9" s="1" t="s">
         <v>64</v>
       </c>
-      <c r="G9" s="2">
+      <c r="G9" s="1">
         <v>2632</v>
       </c>
-      <c r="H9" s="2">
-        <v>0</v>
-      </c>
-      <c r="I9" s="3" t="s">
+      <c r="H9" s="1">
+        <v>0</v>
+      </c>
+      <c r="I9" s="1" t="s">
         <v>65</v>
       </c>
-      <c r="J9" s="3" t="s">
+      <c r="J9" s="1" t="s">
         <v>66</v>
       </c>
-      <c r="K9" s="2">
+      <c r="K9" s="1">
         <v>2632</v>
       </c>
-      <c r="L9" s="2">
-        <v>0</v>
-      </c>
-      <c r="M9" s="2">
+      <c r="L9" s="1">
+        <v>0</v>
+      </c>
+      <c r="M9" s="1">
         <v>35571</v>
       </c>
-      <c r="N9" s="3" t="s">
+      <c r="N9" s="1" t="s">
         <v>34</v>
       </c>
-      <c r="O9" s="2">
+      <c r="O9" s="1">
         <v>1</v>
       </c>
-      <c r="P9" s="3" t="s">
-        <v>36</v>
-      </c>
-      <c r="Q9" s="3" t="s">
-        <v>36</v>
-      </c>
-      <c r="R9" s="3" t="s">
-        <v>36</v>
-      </c>
-      <c r="S9" s="3" t="s">
+      <c r="P9" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="Q9" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="R9" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="S9" s="1" t="s">
         <v>67</v>
       </c>
-      <c r="T9" s="3" t="s">
+      <c r="T9" s="1" t="s">
         <v>67</v>
       </c>
-      <c r="U9" s="3" t="s">
+      <c r="U9" s="1" t="s">
         <v>67</v>
       </c>
-      <c r="V9" s="2" t="b">
+      <c r="V9" s="1" t="b">
         <v>1</v>
       </c>
     </row>
     <row r="10" spans="1:22" x14ac:dyDescent="0.25">
-      <c r="A10" s="1">
-        <v>0</v>
-      </c>
-      <c r="B10" s="1">
+      <c r="A10">
+        <v>0</v>
+      </c>
+      <c r="B10">
         <v>1</v>
       </c>
-      <c r="C10" s="1">
+      <c r="C10">
         <v>2</v>
       </c>
       <c r="D10">
         <v>3</v>
       </c>
-      <c r="E10" s="1">
+      <c r="E10">
         <v>4</v>
       </c>
-      <c r="F10" s="1">
+      <c r="F10">
         <v>5</v>
       </c>
       <c r="G10">
@@ -3874,10 +3866,10 @@
       <c r="H10">
         <v>7</v>
       </c>
-      <c r="I10" s="1">
+      <c r="I10">
         <v>8</v>
       </c>
-      <c r="J10" s="1">
+      <c r="J10">
         <v>9</v>
       </c>
       <c r="K10">
@@ -3889,28 +3881,28 @@
       <c r="M10">
         <v>12</v>
       </c>
-      <c r="N10" s="1">
+      <c r="N10">
         <v>14</v>
       </c>
       <c r="O10">
         <v>15</v>
       </c>
-      <c r="P10" s="1">
+      <c r="P10">
         <v>16</v>
       </c>
-      <c r="Q10" s="1">
+      <c r="Q10">
         <v>17</v>
       </c>
-      <c r="R10" s="1">
+      <c r="R10">
         <v>17</v>
       </c>
-      <c r="S10" s="1">
+      <c r="S10">
         <v>18</v>
       </c>
-      <c r="T10" s="1">
+      <c r="T10">
         <v>19</v>
       </c>
-      <c r="U10" s="1">
+      <c r="U10">
         <v>20</v>
       </c>
       <c r="V10">
@@ -3927,7 +3919,7 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C481CE19-3723-4C9C-82D1-618AC20CFFBD}">
-  <dimension ref="A2:Z10"/>
+  <dimension ref="A2:C10"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="G14" sqref="G14"/>
@@ -3939,198 +3931,102 @@
     <col min="2" max="3" width="11" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="1:26" x14ac:dyDescent="0.25">
-      <c r="A2" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="B2" s="1" t="s">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>0</v>
+      </c>
+      <c r="B2" t="s">
         <v>82</v>
       </c>
-      <c r="C2" s="1" t="s">
+      <c r="C2" t="s">
         <v>84</v>
       </c>
-      <c r="E2" s="1"/>
-      <c r="F2" s="1"/>
-      <c r="I2" s="1"/>
-      <c r="J2" s="1"/>
-      <c r="N2" s="1"/>
-      <c r="P2" s="1"/>
-      <c r="Q2" s="1"/>
-      <c r="R2" s="1"/>
-      <c r="S2" s="1"/>
-      <c r="T2" s="1"/>
-      <c r="U2" s="1"/>
-      <c r="Z2" s="1"/>
-    </row>
-    <row r="3" spans="1:26" x14ac:dyDescent="0.25">
-      <c r="A3" s="1" t="s">
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
         <v>76</v>
       </c>
-      <c r="B3" s="1" t="s">
+      <c r="B3" t="s">
         <v>77</v>
       </c>
-      <c r="C3" s="1" t="s">
-        <v>36</v>
-      </c>
-      <c r="E3" s="1"/>
-      <c r="F3" s="1"/>
-      <c r="I3" s="1"/>
-      <c r="J3" s="1"/>
-      <c r="N3" s="1"/>
-      <c r="P3" s="1"/>
-      <c r="Q3" s="1"/>
-      <c r="R3" s="1"/>
-      <c r="S3" s="1"/>
-      <c r="T3" s="1"/>
-      <c r="U3" s="1"/>
-      <c r="Z3" s="1"/>
-    </row>
-    <row r="4" spans="1:26" x14ac:dyDescent="0.25">
-      <c r="A4" s="1" t="s">
+      <c r="C3" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
         <v>76</v>
       </c>
-      <c r="B4" s="1" t="s">
+      <c r="B4" t="s">
         <v>77</v>
       </c>
-      <c r="C4" s="1" t="s">
-        <v>36</v>
-      </c>
-      <c r="E4" s="1"/>
-      <c r="F4" s="1"/>
-      <c r="I4" s="1"/>
-      <c r="J4" s="1"/>
-      <c r="N4" s="1"/>
-      <c r="P4" s="1"/>
-      <c r="Q4" s="1"/>
-      <c r="R4" s="1"/>
-      <c r="S4" s="1"/>
-      <c r="T4" s="1"/>
-      <c r="U4" s="1"/>
-      <c r="Z4" s="1"/>
-    </row>
-    <row r="5" spans="1:26" x14ac:dyDescent="0.25">
-      <c r="A5" s="1" t="s">
+      <c r="C4" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
         <v>76</v>
       </c>
-      <c r="B5" s="1" t="s">
+      <c r="B5" t="s">
         <v>77</v>
       </c>
-      <c r="C5" s="1" t="s">
-        <v>36</v>
-      </c>
-      <c r="E5" s="1"/>
-      <c r="F5" s="1"/>
-      <c r="I5" s="1"/>
-      <c r="J5" s="1"/>
-      <c r="N5" s="1"/>
-      <c r="P5" s="1"/>
-      <c r="Q5" s="1"/>
-      <c r="R5" s="1"/>
-      <c r="S5" s="1"/>
-      <c r="T5" s="1"/>
-      <c r="U5" s="1"/>
-      <c r="Z5" s="1"/>
-    </row>
-    <row r="6" spans="1:26" x14ac:dyDescent="0.25">
-      <c r="A6" s="1" t="s">
+      <c r="C5" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
         <v>76</v>
       </c>
-      <c r="B6" s="1" t="s">
+      <c r="B6" t="s">
         <v>77</v>
       </c>
-      <c r="C6" s="1" t="s">
-        <v>36</v>
-      </c>
-      <c r="E6" s="1"/>
-      <c r="F6" s="1"/>
-      <c r="I6" s="1"/>
-      <c r="J6" s="1"/>
-      <c r="N6" s="1"/>
-      <c r="P6" s="1"/>
-      <c r="Q6" s="1"/>
-      <c r="R6" s="1"/>
-      <c r="S6" s="1"/>
-      <c r="T6" s="1"/>
-      <c r="U6" s="1"/>
-      <c r="Z6" s="1"/>
-    </row>
-    <row r="7" spans="1:26" x14ac:dyDescent="0.25">
-      <c r="A7" s="1" t="s">
+      <c r="C6" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
         <v>76</v>
       </c>
-      <c r="B7" s="1" t="s">
+      <c r="B7" t="s">
         <v>77</v>
       </c>
-      <c r="C7" s="1" t="s">
-        <v>36</v>
-      </c>
-      <c r="E7" s="1"/>
-      <c r="F7" s="1"/>
-      <c r="I7" s="1"/>
-      <c r="J7" s="1"/>
-      <c r="N7" s="1"/>
-      <c r="P7" s="1"/>
-      <c r="Q7" s="1"/>
-      <c r="R7" s="1"/>
-      <c r="S7" s="1"/>
-      <c r="T7" s="1"/>
-      <c r="U7" s="1"/>
-      <c r="Z7" s="1"/>
-    </row>
-    <row r="8" spans="1:26" x14ac:dyDescent="0.25">
-      <c r="A8" s="1" t="s">
+      <c r="C7" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
         <v>76</v>
       </c>
-      <c r="B8" s="1" t="s">
+      <c r="B8" t="s">
         <v>77</v>
       </c>
-      <c r="C8" s="1" t="s">
-        <v>36</v>
-      </c>
-      <c r="E8" s="1"/>
-      <c r="F8" s="1"/>
-      <c r="I8" s="1"/>
-      <c r="J8" s="1"/>
-      <c r="N8" s="1"/>
-      <c r="P8" s="1"/>
-      <c r="Q8" s="1"/>
-      <c r="R8" s="1"/>
-      <c r="S8" s="1"/>
-      <c r="T8" s="1"/>
-      <c r="U8" s="1"/>
-      <c r="Z8" s="1"/>
-    </row>
-    <row r="9" spans="1:26" x14ac:dyDescent="0.25">
-      <c r="A9" s="1" t="s">
+      <c r="C8" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
         <v>76</v>
       </c>
-      <c r="B9" s="1" t="s">
+      <c r="B9" t="s">
         <v>77</v>
       </c>
-      <c r="C9" s="1" t="s">
-        <v>36</v>
-      </c>
-      <c r="E9" s="1"/>
-      <c r="F9" s="1"/>
-      <c r="I9" s="1"/>
-      <c r="J9" s="1"/>
-      <c r="N9" s="1"/>
-      <c r="P9" s="1"/>
-      <c r="Q9" s="1"/>
-      <c r="R9" s="1"/>
-      <c r="S9" s="1"/>
-      <c r="T9" s="1"/>
-      <c r="U9" s="1"/>
-      <c r="Z9" s="1"/>
-    </row>
-    <row r="10" spans="1:26" x14ac:dyDescent="0.25">
-      <c r="A10" s="1" t="s">
+      <c r="C9" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
         <v>76</v>
       </c>
-      <c r="B10" s="1" t="s">
+      <c r="B10" t="s">
         <v>77</v>
       </c>
-      <c r="C10" s="1" t="s">
+      <c r="C10" t="s">
         <v>36</v>
       </c>
     </row>
@@ -4144,10 +4040,10 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7149F118-EA2A-44D9-A747-FC1191EBFB26}">
-  <dimension ref="A1:Z3"/>
+  <dimension ref="A1:N3"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="I7" sqref="I7"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="I1" sqref="I1:I1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4167,7 +4063,7 @@
     <col min="14" max="14" width="5.28515625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -4211,23 +4107,23 @@
         <v>97</v>
       </c>
     </row>
-    <row r="2" spans="1:26" x14ac:dyDescent="0.25">
-      <c r="A2" s="1" t="s">
+    <row r="2" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
         <v>25</v>
       </c>
-      <c r="B2" s="1" t="s">
+      <c r="B2" t="s">
         <v>58</v>
       </c>
-      <c r="C2" s="1" t="s">
+      <c r="C2" t="s">
         <v>75</v>
       </c>
       <c r="D2" t="b">
         <v>1</v>
       </c>
-      <c r="E2" s="1" t="s">
+      <c r="E2" t="s">
         <v>37</v>
       </c>
-      <c r="F2" s="1" t="s">
+      <c r="F2" t="s">
         <v>36</v>
       </c>
       <c r="G2">
@@ -4236,10 +4132,10 @@
       <c r="H2">
         <v>-2147483648</v>
       </c>
-      <c r="I2" s="1" t="s">
+      <c r="I2" t="s">
         <v>38</v>
       </c>
-      <c r="J2" s="1" t="s">
+      <c r="J2" t="s">
         <v>39</v>
       </c>
       <c r="K2">
@@ -4251,66 +4147,53 @@
       <c r="M2">
         <v>1</v>
       </c>
-      <c r="N2" s="1" t="s">
+      <c r="N2" t="s">
         <v>67</v>
       </c>
-      <c r="P2" s="1"/>
-      <c r="Q2" s="1"/>
-      <c r="R2" s="1"/>
-      <c r="S2" s="1"/>
-      <c r="T2" s="1"/>
-      <c r="U2" s="1"/>
-      <c r="Z2" s="1"/>
-    </row>
-    <row r="3" spans="1:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="1">
-        <v>0</v>
-      </c>
-      <c r="B3" s="1">
+    </row>
+    <row r="3" spans="1:14" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A3">
         <v>1</v>
       </c>
-      <c r="C3" s="1">
+      <c r="B3">
         <v>2</v>
       </c>
+      <c r="C3">
+        <v>3</v>
+      </c>
       <c r="D3">
-        <v>3</v>
-      </c>
-      <c r="E3" s="1">
         <v>4</v>
       </c>
-      <c r="F3" s="1">
+      <c r="E3">
         <v>5</v>
       </c>
+      <c r="F3">
+        <v>6</v>
+      </c>
       <c r="G3">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="H3">
-        <v>7</v>
-      </c>
-      <c r="I3" s="1">
         <v>8</v>
       </c>
-      <c r="J3" s="1">
+      <c r="I3">
         <v>9</v>
       </c>
+      <c r="J3">
+        <v>10</v>
+      </c>
       <c r="K3">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="L3">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="M3">
-        <v>12</v>
-      </c>
-      <c r="N3" s="1">
+        <v>13</v>
+      </c>
+      <c r="N3">
         <v>14</v>
       </c>
-      <c r="P3" s="1"/>
-      <c r="Q3" s="1"/>
-      <c r="R3" s="1"/>
-      <c r="S3" s="1"/>
-      <c r="T3" s="1"/>
-      <c r="U3" s="1"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -4322,7 +4205,7 @@
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{84E833E1-0BD5-44A1-8AED-76C2920B21B7}">
-  <dimension ref="A1:Z4"/>
+  <dimension ref="A1:W4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="E25" sqref="E25"/>
@@ -4351,7 +4234,7 @@
     <col min="19" max="19" width="8.42578125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -4421,25 +4304,24 @@
       <c r="W1" t="s">
         <v>93</v>
       </c>
-      <c r="Z1" s="1"/>
-    </row>
-    <row r="2" spans="1:26" x14ac:dyDescent="0.25">
-      <c r="A2" s="1" t="s">
+    </row>
+    <row r="2" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
         <v>25</v>
       </c>
-      <c r="B2" s="1" t="s">
+      <c r="B2" t="s">
         <v>78</v>
       </c>
-      <c r="C2" s="1" t="s">
+      <c r="C2" t="s">
         <v>79</v>
       </c>
       <c r="D2" t="b">
         <v>1</v>
       </c>
-      <c r="E2" s="1" t="s">
-        <v>36</v>
-      </c>
-      <c r="F2" s="1" t="s">
+      <c r="E2" t="s">
+        <v>36</v>
+      </c>
+      <c r="F2" t="s">
         <v>36</v>
       </c>
       <c r="G2">
@@ -4448,10 +4330,10 @@
       <c r="H2">
         <v>-2147483648</v>
       </c>
-      <c r="I2" s="1" t="s">
+      <c r="I2" t="s">
         <v>38</v>
       </c>
-      <c r="J2" s="1" t="s">
+      <c r="J2" t="s">
         <v>39</v>
       </c>
       <c r="K2">
@@ -4463,54 +4345,54 @@
       <c r="M2" t="s">
         <v>36</v>
       </c>
-      <c r="N2" s="1" t="s">
+      <c r="N2" t="s">
         <v>80</v>
       </c>
       <c r="O2">
         <v>0</v>
       </c>
-      <c r="P2" s="1" t="s">
+      <c r="P2" t="s">
         <v>81</v>
       </c>
-      <c r="Q2" s="1" t="s">
-        <v>36</v>
-      </c>
-      <c r="R2" s="1" t="s">
-        <v>36</v>
-      </c>
-      <c r="S2" s="1" t="s">
-        <v>36</v>
-      </c>
-      <c r="T2" s="1" t="b">
-        <v>0</v>
-      </c>
-      <c r="U2" s="1" t="b">
-        <v>0</v>
-      </c>
-      <c r="V2" s="1" t="b">
-        <v>0</v>
-      </c>
-      <c r="W2" s="1" t="b">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="3" spans="1:26" x14ac:dyDescent="0.25">
-      <c r="A3" s="1" t="s">
+      <c r="Q2" t="s">
+        <v>36</v>
+      </c>
+      <c r="R2" t="s">
+        <v>36</v>
+      </c>
+      <c r="S2" t="s">
+        <v>36</v>
+      </c>
+      <c r="T2" t="b">
+        <v>0</v>
+      </c>
+      <c r="U2" t="b">
+        <v>0</v>
+      </c>
+      <c r="V2" t="b">
+        <v>0</v>
+      </c>
+      <c r="W2" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
         <v>25</v>
       </c>
-      <c r="B3" s="1">
+      <c r="B3">
         <v>1713370858.6340001</v>
       </c>
-      <c r="C3" s="1" t="s">
+      <c r="C3" t="s">
         <v>79</v>
       </c>
       <c r="D3" t="b">
         <v>1</v>
       </c>
-      <c r="E3" s="1" t="s">
-        <v>36</v>
-      </c>
-      <c r="F3" s="1" t="s">
+      <c r="E3" t="s">
+        <v>36</v>
+      </c>
+      <c r="F3" t="s">
         <v>36</v>
       </c>
       <c r="G3">
@@ -4519,10 +4401,10 @@
       <c r="H3">
         <v>-2147483648</v>
       </c>
-      <c r="I3" s="1" t="s">
+      <c r="I3" t="s">
         <v>38</v>
       </c>
-      <c r="J3" s="1" t="s">
+      <c r="J3" t="s">
         <v>39</v>
       </c>
       <c r="K3">
@@ -4534,54 +4416,54 @@
       <c r="M3" t="s">
         <v>87</v>
       </c>
-      <c r="N3" s="1">
+      <c r="N3">
         <v>92717</v>
       </c>
       <c r="O3">
         <v>0</v>
       </c>
-      <c r="P3" s="1" t="s">
+      <c r="P3" t="s">
         <v>81</v>
       </c>
-      <c r="Q3" s="1" t="s">
-        <v>36</v>
-      </c>
-      <c r="R3" s="1" t="s">
-        <v>36</v>
-      </c>
-      <c r="S3" s="1" t="s">
-        <v>36</v>
-      </c>
-      <c r="T3" s="1" t="b">
-        <v>0</v>
-      </c>
-      <c r="U3" s="1" t="b">
-        <v>0</v>
-      </c>
-      <c r="V3" s="1" t="b">
-        <v>0</v>
-      </c>
-      <c r="W3" s="1" t="b">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="4" spans="1:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="1">
-        <v>0</v>
-      </c>
-      <c r="B4" s="1">
+      <c r="Q3" t="s">
+        <v>36</v>
+      </c>
+      <c r="R3" t="s">
+        <v>36</v>
+      </c>
+      <c r="S3" t="s">
+        <v>36</v>
+      </c>
+      <c r="T3" t="b">
+        <v>0</v>
+      </c>
+      <c r="U3" t="b">
+        <v>0</v>
+      </c>
+      <c r="V3" t="b">
+        <v>0</v>
+      </c>
+      <c r="W3" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="4" spans="1:23" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A4">
+        <v>0</v>
+      </c>
+      <c r="B4">
         <v>1</v>
       </c>
-      <c r="C4" s="1">
+      <c r="C4">
         <v>2</v>
       </c>
       <c r="D4">
         <v>3</v>
       </c>
-      <c r="E4" s="1">
+      <c r="E4">
         <v>4</v>
       </c>
-      <c r="F4" s="1">
+      <c r="F4">
         <v>5</v>
       </c>
       <c r="G4">
@@ -4590,10 +4472,10 @@
       <c r="H4">
         <v>7</v>
       </c>
-      <c r="I4" s="1">
+      <c r="I4">
         <v>8</v>
       </c>
-      <c r="J4" s="1">
+      <c r="J4">
         <v>9</v>
       </c>
       <c r="K4">
@@ -4605,28 +4487,28 @@
       <c r="M4">
         <v>12</v>
       </c>
-      <c r="N4" s="1">
+      <c r="N4">
         <v>14</v>
       </c>
       <c r="O4">
         <v>15</v>
       </c>
-      <c r="P4" s="1">
+      <c r="P4">
         <v>16</v>
       </c>
-      <c r="Q4" s="1">
+      <c r="Q4">
         <v>17</v>
       </c>
-      <c r="R4" s="1">
+      <c r="R4">
         <v>17</v>
       </c>
-      <c r="S4" s="1">
+      <c r="S4">
         <v>18</v>
       </c>
-      <c r="T4" s="1">
+      <c r="T4">
         <v>19</v>
       </c>
-      <c r="U4" s="1">
+      <c r="U4">
         <v>20</v>
       </c>
       <c r="V4">

</xml_diff>